<commit_message>
Last Update 29-06-2019  8:40:42.73
</commit_message>
<xml_diff>
--- a/2019/Acadamic Log Book OOPS-19_20.xlsx
+++ b/2019/Acadamic Log Book OOPS-19_20.xlsx
@@ -4,27 +4,28 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
     <sheet name="Expected Internal Marks" sheetId="6" state="hidden" r:id="rId2"/>
     <sheet name="Lab Attendance" sheetId="4" r:id="rId3"/>
-    <sheet name="UT-1-Satement" sheetId="7" r:id="rId4"/>
-    <sheet name="Model 1" sheetId="11" r:id="rId5"/>
-    <sheet name="Record Submission Status" sheetId="9" r:id="rId6"/>
+    <sheet name="Slip Test 1" sheetId="12" r:id="rId4"/>
+    <sheet name="UT-1-Satement" sheetId="7" r:id="rId5"/>
+    <sheet name="Model 1" sheetId="11" r:id="rId6"/>
+    <sheet name="Record Submission Status" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Attendance!$AZ$1:$AZ$57</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Expected Internal Marks'!$C$1:$C$56</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Model 1'!$C$1:$C$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Model 1'!$C$1:$C$63</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="189">
   <si>
     <t>S.NO</t>
   </si>
@@ -567,6 +568,30 @@
   </si>
   <si>
     <t xml:space="preserve"> Statement of Marks - Model Exam</t>
+  </si>
+  <si>
+    <t>ASWIN VISHAL</t>
+  </si>
+  <si>
+    <t>RAKSHANDHAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Statement of Marks - Slip Test-I</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>ABSENT</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -720,7 +745,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -766,6 +791,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -949,7 +986,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="195">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1352,62 +1389,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1436,38 +1440,126 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="17" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="2" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1478,61 +1570,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="2" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1549,13 +1586,70 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1949,11 +2043,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BM57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C50" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -1967,41 +2061,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:65" ht="18.75">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="146" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
       <c r="D1" s="37" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="132" t="s">
+      <c r="F1" s="150" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="133"/>
-      <c r="H1" s="133"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="140" t="s">
+      <c r="G1" s="151"/>
+      <c r="H1" s="151"/>
+      <c r="I1" s="152"/>
+      <c r="J1" s="153" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="140"/>
-      <c r="L1" s="140"/>
-      <c r="M1" s="140"/>
-      <c r="N1" s="142" t="s">
+      <c r="K1" s="153"/>
+      <c r="L1" s="153"/>
+      <c r="M1" s="153"/>
+      <c r="N1" s="155" t="s">
         <v>174</v>
       </c>
-      <c r="O1" s="143"/>
-      <c r="P1" s="143"/>
-      <c r="Q1" s="143"/>
-      <c r="R1" s="143"/>
-      <c r="S1" s="143"/>
-      <c r="T1" s="143"/>
-      <c r="U1" s="143"/>
-      <c r="V1" s="143"/>
-      <c r="W1" s="144"/>
+      <c r="O1" s="156"/>
+      <c r="P1" s="156"/>
+      <c r="Q1" s="156"/>
+      <c r="R1" s="156"/>
+      <c r="S1" s="156"/>
+      <c r="T1" s="156"/>
+      <c r="U1" s="156"/>
+      <c r="V1" s="156"/>
+      <c r="W1" s="157"/>
       <c r="X1" s="44"/>
       <c r="Y1" s="44"/>
       <c r="Z1" s="44"/>
@@ -2014,41 +2108,41 @@
       <c r="AG1" s="44"/>
     </row>
     <row r="2" spans="1:65" ht="19.5">
-      <c r="A2" s="154" t="s">
+      <c r="A2" s="143" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="155"/>
-      <c r="C2" s="156"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="145"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="135" t="s">
+      <c r="F2" s="137" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="135"/>
-      <c r="H2" s="135"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="140" t="s">
+      <c r="G2" s="137"/>
+      <c r="H2" s="137"/>
+      <c r="I2" s="137"/>
+      <c r="J2" s="153" t="s">
         <v>74</v>
       </c>
-      <c r="K2" s="140"/>
-      <c r="L2" s="140"/>
-      <c r="M2" s="140"/>
-      <c r="N2" s="141" t="s">
+      <c r="K2" s="153"/>
+      <c r="L2" s="153"/>
+      <c r="M2" s="153"/>
+      <c r="N2" s="154" t="s">
         <v>179</v>
       </c>
-      <c r="O2" s="141"/>
-      <c r="P2" s="141"/>
-      <c r="Q2" s="141"/>
-      <c r="R2" s="141"/>
-      <c r="S2" s="141"/>
-      <c r="T2" s="141"/>
-      <c r="U2" s="141"/>
-      <c r="V2" s="141"/>
-      <c r="W2" s="141"/>
+      <c r="O2" s="154"/>
+      <c r="P2" s="154"/>
+      <c r="Q2" s="154"/>
+      <c r="R2" s="154"/>
+      <c r="S2" s="154"/>
+      <c r="T2" s="154"/>
+      <c r="U2" s="154"/>
+      <c r="V2" s="154"/>
+      <c r="W2" s="154"/>
       <c r="X2" s="44"/>
       <c r="Y2" s="44"/>
       <c r="Z2" s="44"/>
@@ -2061,41 +2155,41 @@
       <c r="AG2" s="44"/>
     </row>
     <row r="3" spans="1:65" ht="18.75">
-      <c r="A3" s="130" t="s">
+      <c r="A3" s="146" t="s">
         <v>175</v>
       </c>
-      <c r="B3" s="131"/>
-      <c r="C3" s="136"/>
+      <c r="B3" s="147"/>
+      <c r="C3" s="148"/>
       <c r="D3" s="43" t="s">
         <v>71</v>
       </c>
       <c r="E3" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="135" t="s">
+      <c r="F3" s="137" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="135"/>
-      <c r="H3" s="135"/>
-      <c r="I3" s="135"/>
-      <c r="J3" s="140" t="s">
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="137"/>
+      <c r="J3" s="153" t="s">
         <v>75</v>
       </c>
-      <c r="K3" s="140"/>
-      <c r="L3" s="140"/>
-      <c r="M3" s="140"/>
-      <c r="N3" s="141" t="s">
+      <c r="K3" s="153"/>
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="154" t="s">
         <v>77</v>
       </c>
-      <c r="O3" s="141"/>
-      <c r="P3" s="141"/>
-      <c r="Q3" s="141"/>
-      <c r="R3" s="141"/>
-      <c r="S3" s="141"/>
-      <c r="T3" s="141"/>
-      <c r="U3" s="141"/>
-      <c r="V3" s="141"/>
-      <c r="W3" s="141"/>
+      <c r="O3" s="154"/>
+      <c r="P3" s="154"/>
+      <c r="Q3" s="154"/>
+      <c r="R3" s="154"/>
+      <c r="S3" s="154"/>
+      <c r="T3" s="154"/>
+      <c r="U3" s="154"/>
+      <c r="V3" s="154"/>
+      <c r="W3" s="154"/>
       <c r="X3" s="45"/>
       <c r="Y3" s="45"/>
       <c r="Z3" s="45"/>
@@ -2108,68 +2202,68 @@
       <c r="AG3" s="45"/>
     </row>
     <row r="4" spans="1:65" ht="18.75">
-      <c r="A4" s="130" t="s">
+      <c r="A4" s="146" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="131"/>
-      <c r="C4" s="136"/>
-      <c r="D4" s="137"/>
-      <c r="E4" s="138"/>
-      <c r="F4" s="138"/>
-      <c r="G4" s="138"/>
-      <c r="H4" s="138"/>
-      <c r="I4" s="138"/>
-      <c r="J4" s="138"/>
-      <c r="K4" s="138"/>
-      <c r="L4" s="138"/>
-      <c r="M4" s="138"/>
-      <c r="N4" s="138"/>
-      <c r="O4" s="138"/>
-      <c r="P4" s="138"/>
-      <c r="Q4" s="138"/>
-      <c r="R4" s="138"/>
-      <c r="S4" s="138"/>
-      <c r="T4" s="138"/>
-      <c r="U4" s="138"/>
-      <c r="V4" s="138"/>
-      <c r="W4" s="139"/>
-      <c r="X4" s="137"/>
-      <c r="Y4" s="138"/>
-      <c r="Z4" s="138"/>
-      <c r="AA4" s="138"/>
-      <c r="AB4" s="138"/>
-      <c r="AC4" s="138"/>
-      <c r="AD4" s="138"/>
-      <c r="AE4" s="138"/>
-      <c r="AF4" s="138"/>
-      <c r="AG4" s="138"/>
-      <c r="AH4" s="138"/>
-      <c r="AI4" s="138"/>
-      <c r="AJ4" s="138"/>
-      <c r="AK4" s="138"/>
-      <c r="AL4" s="138"/>
-      <c r="AM4" s="138"/>
-      <c r="AN4" s="138"/>
-      <c r="AO4" s="138"/>
-      <c r="AP4" s="138"/>
-      <c r="AQ4" s="138"/>
-      <c r="AR4" s="138"/>
-      <c r="AS4" s="139"/>
-      <c r="AT4" s="137"/>
-      <c r="AU4" s="145"/>
-      <c r="AV4" s="145"/>
-      <c r="AW4" s="145"/>
-      <c r="AX4" s="145"/>
-      <c r="AY4" s="145"/>
-      <c r="AZ4" s="145"/>
-      <c r="BA4" s="145"/>
-      <c r="BB4" s="145"/>
-      <c r="BC4" s="145"/>
-      <c r="BD4" s="145"/>
-      <c r="BE4" s="145"/>
-      <c r="BF4" s="145"/>
-      <c r="BG4" s="145"/>
-      <c r="BH4" s="146"/>
+      <c r="B4" s="147"/>
+      <c r="C4" s="148"/>
+      <c r="D4" s="130"/>
+      <c r="E4" s="133"/>
+      <c r="F4" s="133"/>
+      <c r="G4" s="133"/>
+      <c r="H4" s="133"/>
+      <c r="I4" s="133"/>
+      <c r="J4" s="133"/>
+      <c r="K4" s="133"/>
+      <c r="L4" s="133"/>
+      <c r="M4" s="133"/>
+      <c r="N4" s="133"/>
+      <c r="O4" s="133"/>
+      <c r="P4" s="133"/>
+      <c r="Q4" s="133"/>
+      <c r="R4" s="133"/>
+      <c r="S4" s="133"/>
+      <c r="T4" s="133"/>
+      <c r="U4" s="133"/>
+      <c r="V4" s="133"/>
+      <c r="W4" s="134"/>
+      <c r="X4" s="130"/>
+      <c r="Y4" s="133"/>
+      <c r="Z4" s="133"/>
+      <c r="AA4" s="133"/>
+      <c r="AB4" s="133"/>
+      <c r="AC4" s="133"/>
+      <c r="AD4" s="133"/>
+      <c r="AE4" s="133"/>
+      <c r="AF4" s="133"/>
+      <c r="AG4" s="133"/>
+      <c r="AH4" s="133"/>
+      <c r="AI4" s="133"/>
+      <c r="AJ4" s="133"/>
+      <c r="AK4" s="133"/>
+      <c r="AL4" s="133"/>
+      <c r="AM4" s="133"/>
+      <c r="AN4" s="133"/>
+      <c r="AO4" s="133"/>
+      <c r="AP4" s="133"/>
+      <c r="AQ4" s="133"/>
+      <c r="AR4" s="133"/>
+      <c r="AS4" s="134"/>
+      <c r="AT4" s="130"/>
+      <c r="AU4" s="131"/>
+      <c r="AV4" s="131"/>
+      <c r="AW4" s="131"/>
+      <c r="AX4" s="131"/>
+      <c r="AY4" s="131"/>
+      <c r="AZ4" s="131"/>
+      <c r="BA4" s="131"/>
+      <c r="BB4" s="131"/>
+      <c r="BC4" s="131"/>
+      <c r="BD4" s="131"/>
+      <c r="BE4" s="131"/>
+      <c r="BF4" s="131"/>
+      <c r="BG4" s="131"/>
+      <c r="BH4" s="132"/>
       <c r="BI4" s="51"/>
       <c r="BJ4" s="51"/>
       <c r="BK4" s="51"/>
@@ -2177,10 +2271,10 @@
       <c r="BM4" s="51"/>
     </row>
     <row r="5" spans="1:65">
-      <c r="A5" s="157" t="s">
+      <c r="A5" s="149" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="151" t="s">
+      <c r="B5" s="140" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -2260,8 +2354,8 @@
       <c r="BM5" s="51"/>
     </row>
     <row r="6" spans="1:65">
-      <c r="A6" s="157"/>
-      <c r="B6" s="152"/>
+      <c r="A6" s="149"/>
+      <c r="B6" s="141"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -2342,7 +2436,7 @@
       <c r="A7" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="153"/>
+      <c r="B7" s="142"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -6116,10 +6210,10 @@
       <c r="BM55" s="51"/>
     </row>
     <row r="56" spans="1:65">
-      <c r="A56" s="149" t="s">
+      <c r="A56" s="138" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="150"/>
+      <c r="B56" s="139"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f t="shared" ref="D56:Q56" si="0">COUNTIF(D8:D55,"A")</f>
@@ -6371,10 +6465,10 @@
       </c>
     </row>
     <row r="57" spans="1:65">
-      <c r="A57" s="147" t="s">
+      <c r="A57" s="135" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="148"/>
+      <c r="B57" s="136"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(48-D56)</f>
@@ -6627,15 +6721,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AT4:BH4"/>
-    <mergeCell ref="X4:AS4"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A5:A6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="F3:I3"/>
@@ -6647,6 +6732,15 @@
     <mergeCell ref="N2:W2"/>
     <mergeCell ref="N3:W3"/>
     <mergeCell ref="N1:W1"/>
+    <mergeCell ref="AT4:BH4"/>
+    <mergeCell ref="X4:AS4"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6675,72 +6769,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="158" t="s">
+      <c r="A1" s="166" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="158"/>
+      <c r="B1" s="166"/>
       <c r="C1" s="159" t="s">
         <v>73</v>
       </c>
       <c r="D1" s="159"/>
-      <c r="E1" s="143" t="s">
+      <c r="E1" s="156" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="143"/>
-      <c r="G1" s="143"/>
-      <c r="H1" s="144"/>
+      <c r="F1" s="156"/>
+      <c r="G1" s="156"/>
+      <c r="H1" s="157"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="160" t="s">
+      <c r="A2" s="167" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="160"/>
+      <c r="B2" s="167"/>
       <c r="C2" s="159" t="s">
         <v>74</v>
       </c>
       <c r="D2" s="159"/>
-      <c r="E2" s="141" t="s">
+      <c r="E2" s="154" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="141"/>
-      <c r="G2" s="141"/>
-      <c r="H2" s="141"/>
+      <c r="F2" s="154"/>
+      <c r="G2" s="154"/>
+      <c r="H2" s="154"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="167" t="s">
+      <c r="A3" s="158" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="167"/>
+      <c r="B3" s="158"/>
       <c r="C3" s="159" t="s">
         <v>75</v>
       </c>
       <c r="D3" s="159"/>
-      <c r="E3" s="141" t="s">
+      <c r="E3" s="154" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="141"/>
-      <c r="G3" s="141"/>
-      <c r="H3" s="141"/>
+      <c r="F3" s="154"/>
+      <c r="G3" s="154"/>
+      <c r="H3" s="154"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="161" t="s">
+      <c r="A4" s="160" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="151" t="s">
+      <c r="B4" s="140" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="164" t="s">
+      <c r="C4" s="163" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="165"/>
-      <c r="E4" s="165"/>
-      <c r="F4" s="165"/>
-      <c r="G4" s="165"/>
-      <c r="H4" s="166"/>
+      <c r="D4" s="164"/>
+      <c r="E4" s="164"/>
+      <c r="F4" s="164"/>
+      <c r="G4" s="164"/>
+      <c r="H4" s="165"/>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A5" s="162"/>
-      <c r="B5" s="152"/>
+      <c r="A5" s="161"/>
+      <c r="B5" s="141"/>
       <c r="C5" s="38" t="s">
         <v>62</v>
       </c>
@@ -6761,8 +6855,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="163"/>
-      <c r="B6" s="153"/>
+      <c r="A6" s="162"/>
+      <c r="B6" s="142"/>
       <c r="C6" s="28">
         <v>50</v>
       </c>
@@ -7887,10 +7981,10 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="149" t="s">
+      <c r="A55" s="138" t="s">
         <v>65</v>
       </c>
-      <c r="B55" s="150"/>
+      <c r="B55" s="139"/>
       <c r="C55" s="37">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>38</v>
@@ -7905,10 +7999,10 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="147" t="s">
+      <c r="A56" s="135" t="s">
         <v>66</v>
       </c>
-      <c r="B56" s="148"/>
+      <c r="B56" s="136"/>
       <c r="C56" s="37">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>10</v>
@@ -7923,10 +8017,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="147" t="s">
+      <c r="A57" s="135" t="s">
         <v>67</v>
       </c>
-      <c r="B57" s="148"/>
+      <c r="B57" s="136"/>
       <c r="C57" s="37">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>0</v>
@@ -7941,10 +8035,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="147" t="s">
+      <c r="A58" s="135" t="s">
         <v>68</v>
       </c>
-      <c r="B58" s="148"/>
+      <c r="B58" s="136"/>
       <c r="C58" s="29">
         <f>(C55/48)*100</f>
         <v>79.166666666666657</v>
@@ -7960,35 +8054,35 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:H4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:G54 D24:D54 D7:D22 C7:C47 C49:C54">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E54">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E54">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8015,204 +8109,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18.75">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="146" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
+      <c r="B1" s="147"/>
+      <c r="C1" s="147"/>
       <c r="D1" s="37" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="132" t="s">
+      <c r="F1" s="150" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="133"/>
-      <c r="H1" s="133"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="140" t="s">
+      <c r="G1" s="151"/>
+      <c r="H1" s="151"/>
+      <c r="I1" s="152"/>
+      <c r="J1" s="153" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="140"/>
-      <c r="L1" s="188" t="s">
+      <c r="K1" s="153"/>
+      <c r="L1" s="168" t="s">
         <v>176</v>
       </c>
-      <c r="M1" s="189"/>
-      <c r="N1" s="189"/>
-      <c r="O1" s="189"/>
-      <c r="P1" s="189"/>
-      <c r="Q1" s="189"/>
-      <c r="R1" s="189"/>
-      <c r="S1" s="189"/>
-      <c r="T1" s="189"/>
-      <c r="U1" s="189"/>
-      <c r="V1" s="189"/>
-      <c r="W1" s="189"/>
-      <c r="X1" s="189"/>
-      <c r="Y1" s="189"/>
-      <c r="Z1" s="189"/>
+      <c r="M1" s="169"/>
+      <c r="N1" s="169"/>
+      <c r="O1" s="169"/>
+      <c r="P1" s="169"/>
+      <c r="Q1" s="169"/>
+      <c r="R1" s="169"/>
+      <c r="S1" s="169"/>
+      <c r="T1" s="169"/>
+      <c r="U1" s="169"/>
+      <c r="V1" s="169"/>
+      <c r="W1" s="169"/>
+      <c r="X1" s="169"/>
+      <c r="Y1" s="169"/>
+      <c r="Z1" s="169"/>
     </row>
     <row r="2" spans="1:27" ht="19.5">
-      <c r="A2" s="154" t="s">
+      <c r="A2" s="143" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="155"/>
-      <c r="C2" s="156"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="145"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="135" t="s">
+      <c r="F2" s="137" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="135"/>
-      <c r="H2" s="135"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="140" t="s">
+      <c r="G2" s="137"/>
+      <c r="H2" s="137"/>
+      <c r="I2" s="137"/>
+      <c r="J2" s="153" t="s">
         <v>74</v>
       </c>
-      <c r="K2" s="140"/>
-      <c r="L2" s="188" t="s">
+      <c r="K2" s="153"/>
+      <c r="L2" s="168" t="s">
         <v>177</v>
       </c>
-      <c r="M2" s="189"/>
-      <c r="N2" s="189"/>
-      <c r="O2" s="189"/>
-      <c r="P2" s="189"/>
-      <c r="Q2" s="189"/>
-      <c r="R2" s="189"/>
-      <c r="S2" s="189"/>
-      <c r="T2" s="189"/>
-      <c r="U2" s="189"/>
-      <c r="V2" s="189"/>
-      <c r="W2" s="189"/>
-      <c r="X2" s="189"/>
-      <c r="Y2" s="189"/>
-      <c r="Z2" s="189"/>
+      <c r="M2" s="169"/>
+      <c r="N2" s="169"/>
+      <c r="O2" s="169"/>
+      <c r="P2" s="169"/>
+      <c r="Q2" s="169"/>
+      <c r="R2" s="169"/>
+      <c r="S2" s="169"/>
+      <c r="T2" s="169"/>
+      <c r="U2" s="169"/>
+      <c r="V2" s="169"/>
+      <c r="W2" s="169"/>
+      <c r="X2" s="169"/>
+      <c r="Y2" s="169"/>
+      <c r="Z2" s="169"/>
     </row>
     <row r="3" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A3" s="173" t="s">
+      <c r="A3" s="180" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="174"/>
-      <c r="C3" s="175"/>
+      <c r="B3" s="181"/>
+      <c r="C3" s="182"/>
       <c r="D3" s="43" t="s">
         <v>71</v>
       </c>
       <c r="E3" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="185" t="s">
+      <c r="F3" s="175" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="185"/>
-      <c r="H3" s="185"/>
-      <c r="I3" s="185"/>
-      <c r="J3" s="181" t="s">
+      <c r="G3" s="175"/>
+      <c r="H3" s="175"/>
+      <c r="I3" s="175"/>
+      <c r="J3" s="186" t="s">
         <v>75</v>
       </c>
-      <c r="K3" s="181"/>
-      <c r="L3" s="188" t="s">
+      <c r="K3" s="186"/>
+      <c r="L3" s="168" t="s">
         <v>77</v>
       </c>
-      <c r="M3" s="189"/>
-      <c r="N3" s="189"/>
-      <c r="O3" s="189"/>
-      <c r="P3" s="189"/>
-      <c r="Q3" s="189"/>
-      <c r="R3" s="189"/>
-      <c r="S3" s="189"/>
-      <c r="T3" s="189"/>
-      <c r="U3" s="189"/>
-      <c r="V3" s="189"/>
-      <c r="W3" s="189"/>
-      <c r="X3" s="189"/>
-      <c r="Y3" s="189"/>
-      <c r="Z3" s="189"/>
+      <c r="M3" s="169"/>
+      <c r="N3" s="169"/>
+      <c r="O3" s="169"/>
+      <c r="P3" s="169"/>
+      <c r="Q3" s="169"/>
+      <c r="R3" s="169"/>
+      <c r="S3" s="169"/>
+      <c r="T3" s="169"/>
+      <c r="U3" s="169"/>
+      <c r="V3" s="169"/>
+      <c r="W3" s="169"/>
+      <c r="X3" s="169"/>
+      <c r="Y3" s="169"/>
+      <c r="Z3" s="169"/>
     </row>
     <row r="4" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A4" s="176"/>
-      <c r="B4" s="177"/>
-      <c r="C4" s="178"/>
-      <c r="D4" s="179"/>
-      <c r="E4" s="180"/>
-      <c r="F4" s="180"/>
-      <c r="G4" s="180"/>
-      <c r="H4" s="180"/>
-      <c r="I4" s="180"/>
-      <c r="J4" s="180"/>
-      <c r="K4" s="180"/>
-      <c r="L4" s="179"/>
-      <c r="M4" s="180"/>
-      <c r="N4" s="180"/>
-      <c r="O4" s="180"/>
-      <c r="P4" s="180"/>
-      <c r="Q4" s="180"/>
-      <c r="R4" s="180"/>
-      <c r="S4" s="180"/>
-      <c r="T4" s="186"/>
-      <c r="U4" s="187"/>
-      <c r="V4" s="187"/>
-      <c r="W4" s="187"/>
-      <c r="X4" s="187"/>
-      <c r="Y4" s="187"/>
-      <c r="Z4" s="187"/>
-      <c r="AA4" s="187"/>
+      <c r="A4" s="183"/>
+      <c r="B4" s="184"/>
+      <c r="C4" s="185"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="171"/>
+      <c r="F4" s="171"/>
+      <c r="G4" s="171"/>
+      <c r="H4" s="171"/>
+      <c r="I4" s="171"/>
+      <c r="J4" s="171"/>
+      <c r="K4" s="171"/>
+      <c r="L4" s="170"/>
+      <c r="M4" s="171"/>
+      <c r="N4" s="171"/>
+      <c r="O4" s="171"/>
+      <c r="P4" s="171"/>
+      <c r="Q4" s="171"/>
+      <c r="R4" s="171"/>
+      <c r="S4" s="171"/>
+      <c r="T4" s="178"/>
+      <c r="U4" s="179"/>
+      <c r="V4" s="179"/>
+      <c r="W4" s="179"/>
+      <c r="X4" s="179"/>
+      <c r="Y4" s="179"/>
+      <c r="Z4" s="179"/>
+      <c r="AA4" s="179"/>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="161" t="s">
+      <c r="A5" s="160" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="151" t="s">
+      <c r="B5" s="140" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="168" t="s">
+      <c r="D5" s="187" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="169"/>
-      <c r="F5" s="169"/>
-      <c r="G5" s="170"/>
-      <c r="H5" s="171" t="s">
+      <c r="E5" s="188"/>
+      <c r="F5" s="188"/>
+      <c r="G5" s="189"/>
+      <c r="H5" s="176" t="s">
         <v>64</v>
       </c>
-      <c r="I5" s="172"/>
-      <c r="J5" s="172"/>
-      <c r="K5" s="172"/>
-      <c r="L5" s="171" t="s">
+      <c r="I5" s="177"/>
+      <c r="J5" s="177"/>
+      <c r="K5" s="177"/>
+      <c r="L5" s="176" t="s">
         <v>69</v>
       </c>
-      <c r="M5" s="172"/>
-      <c r="N5" s="172"/>
-      <c r="O5" s="172"/>
-      <c r="P5" s="182" t="s">
+      <c r="M5" s="177"/>
+      <c r="N5" s="177"/>
+      <c r="O5" s="177"/>
+      <c r="P5" s="172" t="s">
         <v>91</v>
       </c>
-      <c r="Q5" s="183"/>
-      <c r="R5" s="183"/>
-      <c r="S5" s="184"/>
-      <c r="T5" s="157" t="s">
+      <c r="Q5" s="173"/>
+      <c r="R5" s="173"/>
+      <c r="S5" s="174"/>
+      <c r="T5" s="149" t="s">
         <v>110</v>
       </c>
-      <c r="U5" s="157"/>
-      <c r="V5" s="157"/>
-      <c r="W5" s="157"/>
-      <c r="X5" s="157" t="s">
+      <c r="U5" s="149"/>
+      <c r="V5" s="149"/>
+      <c r="W5" s="149"/>
+      <c r="X5" s="149" t="s">
         <v>111</v>
       </c>
-      <c r="Y5" s="157"/>
-      <c r="Z5" s="157"/>
-      <c r="AA5" s="157"/>
+      <c r="Y5" s="149"/>
+      <c r="Z5" s="149"/>
+      <c r="AA5" s="149"/>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="162"/>
-      <c r="B6" s="152"/>
+      <c r="A6" s="161"/>
+      <c r="B6" s="141"/>
       <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
@@ -8250,8 +8344,8 @@
       <c r="AA6" s="85"/>
     </row>
     <row r="7" spans="1:27">
-      <c r="A7" s="162"/>
-      <c r="B7" s="152"/>
+      <c r="A7" s="161"/>
+      <c r="B7" s="141"/>
       <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
@@ -8289,8 +8383,8 @@
       <c r="AA7" s="85"/>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1">
-      <c r="A8" s="163"/>
-      <c r="B8" s="153"/>
+      <c r="A8" s="162"/>
+      <c r="B8" s="142"/>
       <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
@@ -9912,10 +10006,10 @@
       <c r="AA56" s="85"/>
     </row>
     <row r="57" spans="1:27">
-      <c r="A57" s="149" t="s">
+      <c r="A57" s="138" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="150"/>
+      <c r="B57" s="139"/>
       <c r="C57" s="13"/>
       <c r="D57" s="17">
         <f>COUNTIF(D9:D56,"A")</f>
@@ -10015,10 +10109,10 @@
       </c>
     </row>
     <row r="58" spans="1:27">
-      <c r="A58" s="147" t="s">
+      <c r="A58" s="135" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="148"/>
+      <c r="B58" s="136"/>
       <c r="C58" s="13"/>
       <c r="D58" s="17">
         <f>(48-D57)</f>
@@ -10119,6 +10213,24 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A3:C4"/>
+    <mergeCell ref="D4:K4"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="T4:AA4"/>
     <mergeCell ref="L1:Z1"/>
     <mergeCell ref="L2:Z2"/>
     <mergeCell ref="L3:Z3"/>
@@ -10126,24 +10238,6 @@
     <mergeCell ref="X5:AA5"/>
     <mergeCell ref="T5:W5"/>
     <mergeCell ref="P5:S5"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="L5:O5"/>
-    <mergeCell ref="T4:AA4"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="A3:C4"/>
-    <mergeCell ref="D4:K4"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="A57:B57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -10151,6 +10245,819 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" style="60" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="60" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="60" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" style="70" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="60"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="191" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="191"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="191"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="192" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="192"/>
+      <c r="C2" s="192"/>
+      <c r="D2" s="192"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="192" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="192"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="192"/>
+    </row>
+    <row r="4" spans="1:4" s="74" customFormat="1" ht="28.5">
+      <c r="A4" s="72" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="71" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="74" customFormat="1" ht="28.5">
+      <c r="A5" s="72" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="71" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" s="73" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="71" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="74" customFormat="1">
+      <c r="A6" s="72" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="71" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="75">
+        <v>43644</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="65" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="74" customFormat="1">
+      <c r="A8" s="57">
+        <v>1</v>
+      </c>
+      <c r="B8" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="61">
+        <v>14</v>
+      </c>
+      <c r="D8" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="74" customFormat="1">
+      <c r="A9" s="57">
+        <v>2</v>
+      </c>
+      <c r="B9" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="62">
+        <v>10</v>
+      </c>
+      <c r="D9" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="74" customFormat="1">
+      <c r="A10" s="57">
+        <v>3</v>
+      </c>
+      <c r="B10" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="61">
+        <v>14</v>
+      </c>
+      <c r="D10" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="74" customFormat="1">
+      <c r="A11" s="57">
+        <v>4</v>
+      </c>
+      <c r="B11" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="61">
+        <v>12</v>
+      </c>
+      <c r="D11" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="74" customFormat="1">
+      <c r="A12" s="57">
+        <v>5</v>
+      </c>
+      <c r="B12" s="76" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="61">
+        <v>14</v>
+      </c>
+      <c r="D12" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="74" customFormat="1">
+      <c r="A13" s="57">
+        <v>6</v>
+      </c>
+      <c r="B13" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="61">
+        <v>11</v>
+      </c>
+      <c r="D13" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="74" customFormat="1">
+      <c r="A14" s="57">
+        <v>7</v>
+      </c>
+      <c r="B14" s="76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="61">
+        <v>15</v>
+      </c>
+      <c r="D14" s="196" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="74" customFormat="1">
+      <c r="A15" s="57">
+        <v>8</v>
+      </c>
+      <c r="B15" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="61">
+        <v>14</v>
+      </c>
+      <c r="D15" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="74" customFormat="1">
+      <c r="A16" s="57">
+        <v>9</v>
+      </c>
+      <c r="B16" s="76" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="197" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="74" customFormat="1">
+      <c r="A17" s="57">
+        <v>10</v>
+      </c>
+      <c r="B17" s="76" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="61">
+        <v>12</v>
+      </c>
+      <c r="D17" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="74" customFormat="1">
+      <c r="A18" s="57">
+        <v>11</v>
+      </c>
+      <c r="B18" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="61">
+        <v>17</v>
+      </c>
+      <c r="D18" s="196" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="74" customFormat="1">
+      <c r="A19" s="57">
+        <v>12</v>
+      </c>
+      <c r="B19" s="76" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="61">
+        <v>19</v>
+      </c>
+      <c r="D19" s="196" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="74" customFormat="1">
+      <c r="A20" s="57">
+        <v>13</v>
+      </c>
+      <c r="B20" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="61">
+        <v>14</v>
+      </c>
+      <c r="D20" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="74" customFormat="1">
+      <c r="A21" s="57">
+        <v>14</v>
+      </c>
+      <c r="B21" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="61">
+        <v>11</v>
+      </c>
+      <c r="D21" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="74" customFormat="1">
+      <c r="A22" s="57">
+        <v>15</v>
+      </c>
+      <c r="B22" s="78" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="61">
+        <v>8</v>
+      </c>
+      <c r="D22" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="74" customFormat="1">
+      <c r="A23" s="57">
+        <v>16</v>
+      </c>
+      <c r="B23" s="76" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="61">
+        <v>11</v>
+      </c>
+      <c r="D23" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="74" customFormat="1">
+      <c r="A24" s="57">
+        <v>17</v>
+      </c>
+      <c r="B24" s="76" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="61">
+        <v>12</v>
+      </c>
+      <c r="D24" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="74" customFormat="1">
+      <c r="A25" s="57">
+        <v>18</v>
+      </c>
+      <c r="B25" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="61">
+        <v>7</v>
+      </c>
+      <c r="D25" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="74" customFormat="1">
+      <c r="A26" s="57">
+        <v>19</v>
+      </c>
+      <c r="B26" s="76" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="61">
+        <v>12</v>
+      </c>
+      <c r="D26" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="74" customFormat="1">
+      <c r="A27" s="57">
+        <v>20</v>
+      </c>
+      <c r="B27" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="61">
+        <v>15</v>
+      </c>
+      <c r="D27" s="196" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="74" customFormat="1">
+      <c r="A28" s="57">
+        <v>21</v>
+      </c>
+      <c r="B28" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="61">
+        <v>3</v>
+      </c>
+      <c r="D28" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="74" customFormat="1">
+      <c r="A29" s="57">
+        <v>22</v>
+      </c>
+      <c r="B29" s="76" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="61">
+        <v>16</v>
+      </c>
+      <c r="D29" s="196" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="74" customFormat="1">
+      <c r="A30" s="57">
+        <v>23</v>
+      </c>
+      <c r="B30" s="79" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="61">
+        <v>12</v>
+      </c>
+      <c r="D30" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="74" customFormat="1">
+      <c r="A31" s="57">
+        <v>24</v>
+      </c>
+      <c r="B31" s="80" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="61">
+        <v>13</v>
+      </c>
+      <c r="D31" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="74" customFormat="1">
+      <c r="A32" s="57">
+        <v>25</v>
+      </c>
+      <c r="B32" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="61">
+        <v>9</v>
+      </c>
+      <c r="D32" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="74" customFormat="1">
+      <c r="A33" s="57">
+        <v>26</v>
+      </c>
+      <c r="B33" s="76" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="61">
+        <v>22</v>
+      </c>
+      <c r="D33" s="196" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="74" customFormat="1">
+      <c r="A34" s="57">
+        <v>27</v>
+      </c>
+      <c r="B34" s="80" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="61">
+        <v>3</v>
+      </c>
+      <c r="D34" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="74" customFormat="1">
+      <c r="A35" s="57">
+        <v>28</v>
+      </c>
+      <c r="B35" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="61">
+        <v>22</v>
+      </c>
+      <c r="D35" s="196" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="74" customFormat="1">
+      <c r="A36" s="57">
+        <v>29</v>
+      </c>
+      <c r="B36" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="61">
+        <v>21</v>
+      </c>
+      <c r="D36" s="196" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="74" customFormat="1">
+      <c r="A37" s="57">
+        <v>30</v>
+      </c>
+      <c r="B37" s="76" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="61">
+        <v>4</v>
+      </c>
+      <c r="D37" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="74" customFormat="1">
+      <c r="A38" s="57">
+        <v>31</v>
+      </c>
+      <c r="B38" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="61">
+        <v>21</v>
+      </c>
+      <c r="D38" s="196" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="74" customFormat="1">
+      <c r="A39" s="57">
+        <v>32</v>
+      </c>
+      <c r="B39" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" s="61">
+        <v>20</v>
+      </c>
+      <c r="D39" s="196" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="74" customFormat="1">
+      <c r="A40" s="57">
+        <v>33</v>
+      </c>
+      <c r="B40" s="76" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="61">
+        <v>11</v>
+      </c>
+      <c r="D40" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="74" customFormat="1">
+      <c r="A41" s="57">
+        <v>34</v>
+      </c>
+      <c r="B41" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="61">
+        <v>16</v>
+      </c>
+      <c r="D41" s="196" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="74" customFormat="1">
+      <c r="A42" s="57">
+        <v>35</v>
+      </c>
+      <c r="B42" s="76" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="61">
+        <v>14</v>
+      </c>
+      <c r="D42" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="74" customFormat="1">
+      <c r="A43" s="57">
+        <v>36</v>
+      </c>
+      <c r="B43" s="76" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="197" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="74" customFormat="1">
+      <c r="A44" s="57">
+        <v>37</v>
+      </c>
+      <c r="B44" s="78" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="61">
+        <v>11</v>
+      </c>
+      <c r="D44" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="74" customFormat="1">
+      <c r="A45" s="57">
+        <v>38</v>
+      </c>
+      <c r="B45" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="61">
+        <v>6</v>
+      </c>
+      <c r="D45" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="74" customFormat="1">
+      <c r="A46" s="57">
+        <v>39</v>
+      </c>
+      <c r="B46" s="80" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="61">
+        <v>9</v>
+      </c>
+      <c r="D46" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="74" customFormat="1">
+      <c r="A47" s="57">
+        <v>40</v>
+      </c>
+      <c r="B47" s="76" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" s="61">
+        <v>13</v>
+      </c>
+      <c r="D47" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="74" customFormat="1">
+      <c r="A48" s="57">
+        <v>41</v>
+      </c>
+      <c r="B48" s="76" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="61">
+        <v>1</v>
+      </c>
+      <c r="D48" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="74" customFormat="1">
+      <c r="A49" s="57">
+        <v>42</v>
+      </c>
+      <c r="B49" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" s="61">
+        <v>17</v>
+      </c>
+      <c r="D49" s="196" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="74" customFormat="1">
+      <c r="A50" s="57">
+        <v>43</v>
+      </c>
+      <c r="B50" s="78" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="61">
+        <v>24</v>
+      </c>
+      <c r="D50" s="196" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="74" customFormat="1">
+      <c r="A51" s="57">
+        <v>44</v>
+      </c>
+      <c r="B51" s="78" t="s">
+        <v>43</v>
+      </c>
+      <c r="C51" s="61">
+        <v>19</v>
+      </c>
+      <c r="D51" s="196" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="74" customFormat="1">
+      <c r="A52" s="57">
+        <v>45</v>
+      </c>
+      <c r="B52" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" s="61">
+        <v>9</v>
+      </c>
+      <c r="D52" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="74" customFormat="1">
+      <c r="A53" s="57">
+        <v>46</v>
+      </c>
+      <c r="B53" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53" s="61">
+        <v>17</v>
+      </c>
+      <c r="D53" s="196" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="74" customFormat="1">
+      <c r="A54" s="57">
+        <v>47</v>
+      </c>
+      <c r="B54" s="76" t="s">
+        <v>46</v>
+      </c>
+      <c r="C54" s="61">
+        <v>17</v>
+      </c>
+      <c r="D54" s="196" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="74" customFormat="1">
+      <c r="A55" s="55">
+        <v>48</v>
+      </c>
+      <c r="B55" s="81" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" s="63">
+        <v>17</v>
+      </c>
+      <c r="D55" s="196" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="74" customFormat="1">
+      <c r="A56" s="55">
+        <v>49</v>
+      </c>
+      <c r="B56" s="81" t="s">
+        <v>181</v>
+      </c>
+      <c r="C56" s="63">
+        <v>12</v>
+      </c>
+      <c r="D56" s="195" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="74" customFormat="1">
+      <c r="A57" s="57">
+        <v>50</v>
+      </c>
+      <c r="B57" s="76" t="s">
+        <v>182</v>
+      </c>
+      <c r="C57" s="61">
+        <v>17</v>
+      </c>
+      <c r="D57" s="196" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C8:C57">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D63"/>
   <sheetViews>
@@ -10806,7 +11713,7 @@
     <mergeCell ref="A3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:C55 C8:C23">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10815,7 +11722,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D63"/>
   <sheetViews>
@@ -11665,12 +12572,12 @@
     <mergeCell ref="A58:C58"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:C55">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C55">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11679,7 +12586,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E52"/>
   <sheetViews>
@@ -12483,13 +13390,13 @@
     <mergeCell ref="A3:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:D52">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"Not Submitted"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"Not Completed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Last Update 11-07-2019 16:46:37.90
</commit_message>
<xml_diff>
--- a/2019/Acadamic Log Book OOPS-19_20.xlsx
+++ b/2019/Acadamic Log Book OOPS-19_20.xlsx
@@ -4,28 +4,31 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15600" windowHeight="7950" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
     <sheet name="Expected Internal Marks" sheetId="6" state="hidden" r:id="rId2"/>
     <sheet name="Lab Attendance" sheetId="4" r:id="rId3"/>
-    <sheet name="Slip Test 1" sheetId="12" r:id="rId4"/>
-    <sheet name="UT-1-Satement" sheetId="7" r:id="rId5"/>
-    <sheet name="Model 1" sheetId="11" r:id="rId6"/>
-    <sheet name="Record Submission Status" sheetId="9" r:id="rId7"/>
+    <sheet name="Slip Test 2" sheetId="13" r:id="rId4"/>
+    <sheet name="Slip Test 1" sheetId="12" r:id="rId5"/>
+    <sheet name="UT-1-Satement" sheetId="7" r:id="rId6"/>
+    <sheet name="Model 1" sheetId="11" r:id="rId7"/>
+    <sheet name="Record Submission Status" sheetId="9" r:id="rId8"/>
+    <sheet name="Book Requierd" sheetId="14" r:id="rId9"/>
+    <sheet name="Failiure" sheetId="15" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Attendance!$AZ$1:$AZ$57</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Expected Internal Marks'!$C$1:$C$56</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Model 1'!$C$1:$C$63</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Model 1'!$C$1:$C$63</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="197">
   <si>
     <t>S.NO</t>
   </si>
@@ -592,6 +595,30 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Statement of Marks - Slip Test-II</t>
+  </si>
+  <si>
+    <t>OOPS Book Request</t>
+  </si>
+  <si>
+    <t>Requierd</t>
+  </si>
+  <si>
+    <t>Signature</t>
+  </si>
+  <si>
+    <t>ST -1</t>
+  </si>
+  <si>
+    <t>ST 2</t>
+  </si>
+  <si>
+    <t>Unit Test Coaching</t>
   </si>
 </sst>
 </file>
@@ -602,7 +629,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -741,6 +768,12 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -986,7 +1019,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="204">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1389,29 +1422,80 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="17" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="17" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1440,82 +1524,94 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="2" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="17" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1524,54 +1620,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="2" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="2" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1580,6 +1628,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1587,13 +1638,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1601,7 +1653,43 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -1668,6 +1756,30 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2061,41 +2173,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:65" ht="18.75">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="136" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
       <c r="D1" s="37" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="150" t="s">
+      <c r="F1" s="138" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="151"/>
-      <c r="H1" s="151"/>
-      <c r="I1" s="152"/>
-      <c r="J1" s="153" t="s">
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="140"/>
+      <c r="J1" s="146" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="153"/>
-      <c r="L1" s="153"/>
-      <c r="M1" s="153"/>
-      <c r="N1" s="155" t="s">
+      <c r="K1" s="146"/>
+      <c r="L1" s="146"/>
+      <c r="M1" s="146"/>
+      <c r="N1" s="148" t="s">
         <v>174</v>
       </c>
-      <c r="O1" s="156"/>
-      <c r="P1" s="156"/>
-      <c r="Q1" s="156"/>
-      <c r="R1" s="156"/>
-      <c r="S1" s="156"/>
-      <c r="T1" s="156"/>
-      <c r="U1" s="156"/>
-      <c r="V1" s="156"/>
-      <c r="W1" s="157"/>
+      <c r="O1" s="149"/>
+      <c r="P1" s="149"/>
+      <c r="Q1" s="149"/>
+      <c r="R1" s="149"/>
+      <c r="S1" s="149"/>
+      <c r="T1" s="149"/>
+      <c r="U1" s="149"/>
+      <c r="V1" s="149"/>
+      <c r="W1" s="150"/>
       <c r="X1" s="44"/>
       <c r="Y1" s="44"/>
       <c r="Z1" s="44"/>
@@ -2108,41 +2220,41 @@
       <c r="AG1" s="44"/>
     </row>
     <row r="2" spans="1:65" ht="19.5">
-      <c r="A2" s="143" t="s">
+      <c r="A2" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="144"/>
-      <c r="C2" s="145"/>
+      <c r="B2" s="161"/>
+      <c r="C2" s="162"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="137" t="s">
+      <c r="F2" s="141" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
-      <c r="J2" s="153" t="s">
+      <c r="G2" s="141"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
+      <c r="J2" s="146" t="s">
         <v>74</v>
       </c>
-      <c r="K2" s="153"/>
-      <c r="L2" s="153"/>
-      <c r="M2" s="153"/>
-      <c r="N2" s="154" t="s">
+      <c r="K2" s="146"/>
+      <c r="L2" s="146"/>
+      <c r="M2" s="146"/>
+      <c r="N2" s="147" t="s">
         <v>179</v>
       </c>
-      <c r="O2" s="154"/>
-      <c r="P2" s="154"/>
-      <c r="Q2" s="154"/>
-      <c r="R2" s="154"/>
-      <c r="S2" s="154"/>
-      <c r="T2" s="154"/>
-      <c r="U2" s="154"/>
-      <c r="V2" s="154"/>
-      <c r="W2" s="154"/>
+      <c r="O2" s="147"/>
+      <c r="P2" s="147"/>
+      <c r="Q2" s="147"/>
+      <c r="R2" s="147"/>
+      <c r="S2" s="147"/>
+      <c r="T2" s="147"/>
+      <c r="U2" s="147"/>
+      <c r="V2" s="147"/>
+      <c r="W2" s="147"/>
       <c r="X2" s="44"/>
       <c r="Y2" s="44"/>
       <c r="Z2" s="44"/>
@@ -2155,41 +2267,41 @@
       <c r="AG2" s="44"/>
     </row>
     <row r="3" spans="1:65" ht="18.75">
-      <c r="A3" s="146" t="s">
+      <c r="A3" s="136" t="s">
         <v>175</v>
       </c>
-      <c r="B3" s="147"/>
-      <c r="C3" s="148"/>
+      <c r="B3" s="137"/>
+      <c r="C3" s="142"/>
       <c r="D3" s="43" t="s">
         <v>71</v>
       </c>
       <c r="E3" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="137" t="s">
+      <c r="F3" s="141" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="137"/>
-      <c r="H3" s="137"/>
-      <c r="I3" s="137"/>
-      <c r="J3" s="153" t="s">
+      <c r="G3" s="141"/>
+      <c r="H3" s="141"/>
+      <c r="I3" s="141"/>
+      <c r="J3" s="146" t="s">
         <v>75</v>
       </c>
-      <c r="K3" s="153"/>
-      <c r="L3" s="153"/>
-      <c r="M3" s="153"/>
-      <c r="N3" s="154" t="s">
+      <c r="K3" s="146"/>
+      <c r="L3" s="146"/>
+      <c r="M3" s="146"/>
+      <c r="N3" s="147" t="s">
         <v>77</v>
       </c>
-      <c r="O3" s="154"/>
-      <c r="P3" s="154"/>
-      <c r="Q3" s="154"/>
-      <c r="R3" s="154"/>
-      <c r="S3" s="154"/>
-      <c r="T3" s="154"/>
-      <c r="U3" s="154"/>
-      <c r="V3" s="154"/>
-      <c r="W3" s="154"/>
+      <c r="O3" s="147"/>
+      <c r="P3" s="147"/>
+      <c r="Q3" s="147"/>
+      <c r="R3" s="147"/>
+      <c r="S3" s="147"/>
+      <c r="T3" s="147"/>
+      <c r="U3" s="147"/>
+      <c r="V3" s="147"/>
+      <c r="W3" s="147"/>
       <c r="X3" s="45"/>
       <c r="Y3" s="45"/>
       <c r="Z3" s="45"/>
@@ -2202,68 +2314,68 @@
       <c r="AG3" s="45"/>
     </row>
     <row r="4" spans="1:65" ht="18.75">
-      <c r="A4" s="146" t="s">
+      <c r="A4" s="136" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="147"/>
-      <c r="C4" s="148"/>
-      <c r="D4" s="130"/>
-      <c r="E4" s="133"/>
-      <c r="F4" s="133"/>
-      <c r="G4" s="133"/>
-      <c r="H4" s="133"/>
-      <c r="I4" s="133"/>
-      <c r="J4" s="133"/>
-      <c r="K4" s="133"/>
-      <c r="L4" s="133"/>
-      <c r="M4" s="133"/>
-      <c r="N4" s="133"/>
-      <c r="O4" s="133"/>
-      <c r="P4" s="133"/>
-      <c r="Q4" s="133"/>
-      <c r="R4" s="133"/>
-      <c r="S4" s="133"/>
-      <c r="T4" s="133"/>
-      <c r="U4" s="133"/>
-      <c r="V4" s="133"/>
-      <c r="W4" s="134"/>
-      <c r="X4" s="130"/>
-      <c r="Y4" s="133"/>
-      <c r="Z4" s="133"/>
-      <c r="AA4" s="133"/>
-      <c r="AB4" s="133"/>
-      <c r="AC4" s="133"/>
-      <c r="AD4" s="133"/>
-      <c r="AE4" s="133"/>
-      <c r="AF4" s="133"/>
-      <c r="AG4" s="133"/>
-      <c r="AH4" s="133"/>
-      <c r="AI4" s="133"/>
-      <c r="AJ4" s="133"/>
-      <c r="AK4" s="133"/>
-      <c r="AL4" s="133"/>
-      <c r="AM4" s="133"/>
-      <c r="AN4" s="133"/>
-      <c r="AO4" s="133"/>
-      <c r="AP4" s="133"/>
-      <c r="AQ4" s="133"/>
-      <c r="AR4" s="133"/>
-      <c r="AS4" s="134"/>
-      <c r="AT4" s="130"/>
-      <c r="AU4" s="131"/>
-      <c r="AV4" s="131"/>
-      <c r="AW4" s="131"/>
-      <c r="AX4" s="131"/>
-      <c r="AY4" s="131"/>
-      <c r="AZ4" s="131"/>
-      <c r="BA4" s="131"/>
-      <c r="BB4" s="131"/>
-      <c r="BC4" s="131"/>
-      <c r="BD4" s="131"/>
-      <c r="BE4" s="131"/>
-      <c r="BF4" s="131"/>
-      <c r="BG4" s="131"/>
-      <c r="BH4" s="132"/>
+      <c r="B4" s="137"/>
+      <c r="C4" s="142"/>
+      <c r="D4" s="143"/>
+      <c r="E4" s="144"/>
+      <c r="F4" s="144"/>
+      <c r="G4" s="144"/>
+      <c r="H4" s="144"/>
+      <c r="I4" s="144"/>
+      <c r="J4" s="144"/>
+      <c r="K4" s="144"/>
+      <c r="L4" s="144"/>
+      <c r="M4" s="144"/>
+      <c r="N4" s="144"/>
+      <c r="O4" s="144"/>
+      <c r="P4" s="144"/>
+      <c r="Q4" s="144"/>
+      <c r="R4" s="144"/>
+      <c r="S4" s="144"/>
+      <c r="T4" s="144"/>
+      <c r="U4" s="144"/>
+      <c r="V4" s="144"/>
+      <c r="W4" s="145"/>
+      <c r="X4" s="143"/>
+      <c r="Y4" s="144"/>
+      <c r="Z4" s="144"/>
+      <c r="AA4" s="144"/>
+      <c r="AB4" s="144"/>
+      <c r="AC4" s="144"/>
+      <c r="AD4" s="144"/>
+      <c r="AE4" s="144"/>
+      <c r="AF4" s="144"/>
+      <c r="AG4" s="144"/>
+      <c r="AH4" s="144"/>
+      <c r="AI4" s="144"/>
+      <c r="AJ4" s="144"/>
+      <c r="AK4" s="144"/>
+      <c r="AL4" s="144"/>
+      <c r="AM4" s="144"/>
+      <c r="AN4" s="144"/>
+      <c r="AO4" s="144"/>
+      <c r="AP4" s="144"/>
+      <c r="AQ4" s="144"/>
+      <c r="AR4" s="144"/>
+      <c r="AS4" s="145"/>
+      <c r="AT4" s="143"/>
+      <c r="AU4" s="151"/>
+      <c r="AV4" s="151"/>
+      <c r="AW4" s="151"/>
+      <c r="AX4" s="151"/>
+      <c r="AY4" s="151"/>
+      <c r="AZ4" s="151"/>
+      <c r="BA4" s="151"/>
+      <c r="BB4" s="151"/>
+      <c r="BC4" s="151"/>
+      <c r="BD4" s="151"/>
+      <c r="BE4" s="151"/>
+      <c r="BF4" s="151"/>
+      <c r="BG4" s="151"/>
+      <c r="BH4" s="152"/>
       <c r="BI4" s="51"/>
       <c r="BJ4" s="51"/>
       <c r="BK4" s="51"/>
@@ -2271,10 +2383,10 @@
       <c r="BM4" s="51"/>
     </row>
     <row r="5" spans="1:65">
-      <c r="A5" s="149" t="s">
+      <c r="A5" s="163" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="140" t="s">
+      <c r="B5" s="157" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -2354,8 +2466,8 @@
       <c r="BM5" s="51"/>
     </row>
     <row r="6" spans="1:65">
-      <c r="A6" s="149"/>
-      <c r="B6" s="141"/>
+      <c r="A6" s="163"/>
+      <c r="B6" s="158"/>
       <c r="C6" s="9" t="s">
         <v>48</v>
       </c>
@@ -2436,7 +2548,7 @@
       <c r="A7" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="142"/>
+      <c r="B7" s="159"/>
       <c r="C7" s="10" t="s">
         <v>49</v>
       </c>
@@ -6210,10 +6322,10 @@
       <c r="BM55" s="51"/>
     </row>
     <row r="56" spans="1:65">
-      <c r="A56" s="138" t="s">
+      <c r="A56" s="155" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="139"/>
+      <c r="B56" s="156"/>
       <c r="C56" s="13"/>
       <c r="D56" s="12">
         <f t="shared" ref="D56:Q56" si="0">COUNTIF(D8:D55,"A")</f>
@@ -6465,10 +6577,10 @@
       </c>
     </row>
     <row r="57" spans="1:65">
-      <c r="A57" s="135" t="s">
+      <c r="A57" s="153" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="136"/>
+      <c r="B57" s="154"/>
       <c r="C57" s="13"/>
       <c r="D57" s="12">
         <f>(48-D56)</f>
@@ -6721,6 +6833,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AT4:BH4"/>
+    <mergeCell ref="X4:AS4"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A5:A6"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="F3:I3"/>
@@ -6732,18 +6853,319 @@
     <mergeCell ref="N2:W2"/>
     <mergeCell ref="N3:W3"/>
     <mergeCell ref="N1:W1"/>
-    <mergeCell ref="AT4:BH4"/>
-    <mergeCell ref="X4:AS4"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" style="60" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="60" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" style="60" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" style="203" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="60"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" customHeight="1">
+      <c r="A1" s="196" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="196"/>
+      <c r="C1" s="196"/>
+      <c r="D1" s="196"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1">
+      <c r="A2" s="197" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="197"/>
+      <c r="C2" s="197"/>
+      <c r="D2" s="197"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1">
+      <c r="A3" s="197" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="197"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>195</v>
+      </c>
+      <c r="D4" s="57" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="74" customFormat="1">
+      <c r="A5" s="57">
+        <v>1</v>
+      </c>
+      <c r="B5" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>189</v>
+      </c>
+      <c r="D5" s="61">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="74" customFormat="1">
+      <c r="A6" s="57">
+        <v>2</v>
+      </c>
+      <c r="B6" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="62">
+        <v>11</v>
+      </c>
+      <c r="D6" s="62">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="74" customFormat="1">
+      <c r="A7" s="57">
+        <v>3</v>
+      </c>
+      <c r="B7" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="61">
+        <v>12</v>
+      </c>
+      <c r="D7" s="61">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="74" customFormat="1">
+      <c r="A8" s="57">
+        <v>4</v>
+      </c>
+      <c r="B8" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="61">
+        <v>14</v>
+      </c>
+      <c r="D8" s="61">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="74" customFormat="1">
+      <c r="A9" s="57">
+        <v>5</v>
+      </c>
+      <c r="B9" s="76" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="62">
+        <v>5</v>
+      </c>
+      <c r="D9" s="62" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="74" customFormat="1">
+      <c r="A10" s="57">
+        <v>6</v>
+      </c>
+      <c r="B10" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="61">
+        <v>16</v>
+      </c>
+      <c r="D10" s="61">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="74" customFormat="1">
+      <c r="A11" s="57">
+        <v>7</v>
+      </c>
+      <c r="B11" s="78" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="61">
+        <v>14</v>
+      </c>
+      <c r="D11" s="61">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="74" customFormat="1">
+      <c r="A12" s="57">
+        <v>8</v>
+      </c>
+      <c r="B12" s="76" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="61">
+        <v>16</v>
+      </c>
+      <c r="D12" s="61">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="74" customFormat="1">
+      <c r="A13" s="57">
+        <v>9</v>
+      </c>
+      <c r="B13" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="61">
+        <v>11</v>
+      </c>
+      <c r="D13" s="61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="74" customFormat="1">
+      <c r="A14" s="57">
+        <v>10</v>
+      </c>
+      <c r="B14" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="61">
+        <v>13</v>
+      </c>
+      <c r="D14" s="61">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="74" customFormat="1">
+      <c r="A15" s="57">
+        <v>11</v>
+      </c>
+      <c r="B15" s="80" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="61">
+        <v>11</v>
+      </c>
+      <c r="D15" s="61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="74" customFormat="1">
+      <c r="A16" s="57">
+        <v>12</v>
+      </c>
+      <c r="B16" s="76" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="61">
+        <v>4</v>
+      </c>
+      <c r="D16" s="61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="74" customFormat="1">
+      <c r="A17" s="57">
+        <v>13</v>
+      </c>
+      <c r="B17" s="76" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="61">
+        <v>16</v>
+      </c>
+      <c r="D17" s="61">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="74" customFormat="1">
+      <c r="A18" s="57">
+        <v>14</v>
+      </c>
+      <c r="B18" s="76" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="62">
+        <v>14</v>
+      </c>
+      <c r="D18" s="62" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="74" customFormat="1">
+      <c r="A19" s="57">
+        <v>15</v>
+      </c>
+      <c r="B19" s="80" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="61">
+        <v>7</v>
+      </c>
+      <c r="D19" s="61">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="74" customFormat="1">
+      <c r="A20" s="57">
+        <v>16</v>
+      </c>
+      <c r="B20" s="76" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="61">
+        <v>14</v>
+      </c>
+      <c r="D20" s="61">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C5:C20">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
+      <formula>18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D20">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+      <formula>18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6769,72 +7191,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="164" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="159" t="s">
+      <c r="B1" s="164"/>
+      <c r="C1" s="165" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="159"/>
-      <c r="E1" s="156" t="s">
+      <c r="D1" s="165"/>
+      <c r="E1" s="149" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="156"/>
-      <c r="G1" s="156"/>
-      <c r="H1" s="157"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="149"/>
+      <c r="H1" s="150"/>
     </row>
     <row r="2" spans="1:8" ht="19.5">
-      <c r="A2" s="167" t="s">
+      <c r="A2" s="166" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="167"/>
-      <c r="C2" s="159" t="s">
+      <c r="B2" s="166"/>
+      <c r="C2" s="165" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="159"/>
-      <c r="E2" s="154" t="s">
+      <c r="D2" s="165"/>
+      <c r="E2" s="147" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="154"/>
-      <c r="G2" s="154"/>
-      <c r="H2" s="154"/>
+      <c r="F2" s="147"/>
+      <c r="G2" s="147"/>
+      <c r="H2" s="147"/>
     </row>
     <row r="3" spans="1:8" ht="17.25">
-      <c r="A3" s="158" t="s">
+      <c r="A3" s="173" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="158"/>
-      <c r="C3" s="159" t="s">
+      <c r="B3" s="173"/>
+      <c r="C3" s="165" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="159"/>
-      <c r="E3" s="154" t="s">
+      <c r="D3" s="165"/>
+      <c r="E3" s="147" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="154"/>
-      <c r="G3" s="154"/>
-      <c r="H3" s="154"/>
+      <c r="F3" s="147"/>
+      <c r="G3" s="147"/>
+      <c r="H3" s="147"/>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1">
-      <c r="A4" s="160" t="s">
+      <c r="A4" s="167" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="140" t="s">
+      <c r="B4" s="157" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="163" t="s">
+      <c r="C4" s="170" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="164"/>
-      <c r="E4" s="164"/>
-      <c r="F4" s="164"/>
-      <c r="G4" s="164"/>
-      <c r="H4" s="165"/>
+      <c r="D4" s="171"/>
+      <c r="E4" s="171"/>
+      <c r="F4" s="171"/>
+      <c r="G4" s="171"/>
+      <c r="H4" s="172"/>
     </row>
     <row r="5" spans="1:8" ht="53.25" customHeight="1">
-      <c r="A5" s="161"/>
-      <c r="B5" s="141"/>
+      <c r="A5" s="168"/>
+      <c r="B5" s="158"/>
       <c r="C5" s="38" t="s">
         <v>62</v>
       </c>
@@ -6855,8 +7277,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="162"/>
-      <c r="B6" s="142"/>
+      <c r="A6" s="169"/>
+      <c r="B6" s="159"/>
       <c r="C6" s="28">
         <v>50</v>
       </c>
@@ -7981,10 +8403,10 @@
       </c>
     </row>
     <row r="55" spans="1:8">
-      <c r="A55" s="138" t="s">
+      <c r="A55" s="155" t="s">
         <v>65</v>
       </c>
-      <c r="B55" s="139"/>
+      <c r="B55" s="156"/>
       <c r="C55" s="37">
         <f>COUNTIF(C7:C54,"&gt;24")</f>
         <v>38</v>
@@ -7999,10 +8421,10 @@
       <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:8">
-      <c r="A56" s="135" t="s">
+      <c r="A56" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="B56" s="136"/>
+      <c r="B56" s="154"/>
       <c r="C56" s="37">
         <f>COUNTIF(C8:C55,"&lt;25")</f>
         <v>10</v>
@@ -8017,10 +8439,10 @@
       <c r="G56" s="13"/>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="135" t="s">
+      <c r="A57" s="153" t="s">
         <v>67</v>
       </c>
-      <c r="B57" s="136"/>
+      <c r="B57" s="154"/>
       <c r="C57" s="37">
         <f>COUNTIF(C9:C56,"AB")</f>
         <v>0</v>
@@ -8035,10 +8457,10 @@
       <c r="G57" s="13"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="135" t="s">
+      <c r="A58" s="153" t="s">
         <v>68</v>
       </c>
-      <c r="B58" s="136"/>
+      <c r="B58" s="154"/>
       <c r="C58" s="29">
         <f>(C55/48)*100</f>
         <v>79.166666666666657</v>
@@ -8054,35 +8476,35 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:H4"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:G54 D24:D54 D7:D22 C7:C47 C49:C54">
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E54">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7:E54">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8109,204 +8531,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18.75">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="136" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="147"/>
-      <c r="C1" s="147"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
       <c r="D1" s="37" t="s">
         <v>54</v>
       </c>
       <c r="E1" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="150" t="s">
+      <c r="F1" s="138" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="151"/>
-      <c r="H1" s="151"/>
-      <c r="I1" s="152"/>
-      <c r="J1" s="153" t="s">
+      <c r="G1" s="139"/>
+      <c r="H1" s="139"/>
+      <c r="I1" s="140"/>
+      <c r="J1" s="146" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="153"/>
-      <c r="L1" s="168" t="s">
+      <c r="K1" s="146"/>
+      <c r="L1" s="191" t="s">
         <v>176</v>
       </c>
-      <c r="M1" s="169"/>
-      <c r="N1" s="169"/>
-      <c r="O1" s="169"/>
-      <c r="P1" s="169"/>
-      <c r="Q1" s="169"/>
-      <c r="R1" s="169"/>
-      <c r="S1" s="169"/>
-      <c r="T1" s="169"/>
-      <c r="U1" s="169"/>
-      <c r="V1" s="169"/>
-      <c r="W1" s="169"/>
-      <c r="X1" s="169"/>
-      <c r="Y1" s="169"/>
-      <c r="Z1" s="169"/>
+      <c r="M1" s="192"/>
+      <c r="N1" s="192"/>
+      <c r="O1" s="192"/>
+      <c r="P1" s="192"/>
+      <c r="Q1" s="192"/>
+      <c r="R1" s="192"/>
+      <c r="S1" s="192"/>
+      <c r="T1" s="192"/>
+      <c r="U1" s="192"/>
+      <c r="V1" s="192"/>
+      <c r="W1" s="192"/>
+      <c r="X1" s="192"/>
+      <c r="Y1" s="192"/>
+      <c r="Z1" s="192"/>
     </row>
     <row r="2" spans="1:27" ht="19.5">
-      <c r="A2" s="143" t="s">
+      <c r="A2" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="144"/>
-      <c r="C2" s="145"/>
+      <c r="B2" s="161"/>
+      <c r="C2" s="162"/>
       <c r="D2" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E2" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="137" t="s">
+      <c r="F2" s="141" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
-      <c r="J2" s="153" t="s">
+      <c r="G2" s="141"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
+      <c r="J2" s="146" t="s">
         <v>74</v>
       </c>
-      <c r="K2" s="153"/>
-      <c r="L2" s="168" t="s">
+      <c r="K2" s="146"/>
+      <c r="L2" s="191" t="s">
         <v>177</v>
       </c>
-      <c r="M2" s="169"/>
-      <c r="N2" s="169"/>
-      <c r="O2" s="169"/>
-      <c r="P2" s="169"/>
-      <c r="Q2" s="169"/>
-      <c r="R2" s="169"/>
-      <c r="S2" s="169"/>
-      <c r="T2" s="169"/>
-      <c r="U2" s="169"/>
-      <c r="V2" s="169"/>
-      <c r="W2" s="169"/>
-      <c r="X2" s="169"/>
-      <c r="Y2" s="169"/>
-      <c r="Z2" s="169"/>
+      <c r="M2" s="192"/>
+      <c r="N2" s="192"/>
+      <c r="O2" s="192"/>
+      <c r="P2" s="192"/>
+      <c r="Q2" s="192"/>
+      <c r="R2" s="192"/>
+      <c r="S2" s="192"/>
+      <c r="T2" s="192"/>
+      <c r="U2" s="192"/>
+      <c r="V2" s="192"/>
+      <c r="W2" s="192"/>
+      <c r="X2" s="192"/>
+      <c r="Y2" s="192"/>
+      <c r="Z2" s="192"/>
     </row>
     <row r="3" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A3" s="180" t="s">
+      <c r="A3" s="179" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="181"/>
-      <c r="C3" s="182"/>
+      <c r="B3" s="180"/>
+      <c r="C3" s="181"/>
       <c r="D3" s="43" t="s">
         <v>71</v>
       </c>
       <c r="E3" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="175" t="s">
+      <c r="F3" s="188" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="175"/>
-      <c r="H3" s="175"/>
-      <c r="I3" s="175"/>
-      <c r="J3" s="186" t="s">
+      <c r="G3" s="188"/>
+      <c r="H3" s="188"/>
+      <c r="I3" s="188"/>
+      <c r="J3" s="187" t="s">
         <v>75</v>
       </c>
-      <c r="K3" s="186"/>
-      <c r="L3" s="168" t="s">
+      <c r="K3" s="187"/>
+      <c r="L3" s="191" t="s">
         <v>77</v>
       </c>
-      <c r="M3" s="169"/>
-      <c r="N3" s="169"/>
-      <c r="O3" s="169"/>
-      <c r="P3" s="169"/>
-      <c r="Q3" s="169"/>
-      <c r="R3" s="169"/>
-      <c r="S3" s="169"/>
-      <c r="T3" s="169"/>
-      <c r="U3" s="169"/>
-      <c r="V3" s="169"/>
-      <c r="W3" s="169"/>
-      <c r="X3" s="169"/>
-      <c r="Y3" s="169"/>
-      <c r="Z3" s="169"/>
+      <c r="M3" s="192"/>
+      <c r="N3" s="192"/>
+      <c r="O3" s="192"/>
+      <c r="P3" s="192"/>
+      <c r="Q3" s="192"/>
+      <c r="R3" s="192"/>
+      <c r="S3" s="192"/>
+      <c r="T3" s="192"/>
+      <c r="U3" s="192"/>
+      <c r="V3" s="192"/>
+      <c r="W3" s="192"/>
+      <c r="X3" s="192"/>
+      <c r="Y3" s="192"/>
+      <c r="Z3" s="192"/>
     </row>
     <row r="4" spans="1:27" ht="18.75" customHeight="1">
-      <c r="A4" s="183"/>
-      <c r="B4" s="184"/>
-      <c r="C4" s="185"/>
-      <c r="D4" s="170"/>
-      <c r="E4" s="171"/>
-      <c r="F4" s="171"/>
-      <c r="G4" s="171"/>
-      <c r="H4" s="171"/>
-      <c r="I4" s="171"/>
-      <c r="J4" s="171"/>
-      <c r="K4" s="171"/>
-      <c r="L4" s="170"/>
-      <c r="M4" s="171"/>
-      <c r="N4" s="171"/>
-      <c r="O4" s="171"/>
-      <c r="P4" s="171"/>
-      <c r="Q4" s="171"/>
-      <c r="R4" s="171"/>
-      <c r="S4" s="171"/>
-      <c r="T4" s="178"/>
-      <c r="U4" s="179"/>
-      <c r="V4" s="179"/>
-      <c r="W4" s="179"/>
-      <c r="X4" s="179"/>
-      <c r="Y4" s="179"/>
-      <c r="Z4" s="179"/>
-      <c r="AA4" s="179"/>
+      <c r="A4" s="182"/>
+      <c r="B4" s="183"/>
+      <c r="C4" s="184"/>
+      <c r="D4" s="185"/>
+      <c r="E4" s="186"/>
+      <c r="F4" s="186"/>
+      <c r="G4" s="186"/>
+      <c r="H4" s="186"/>
+      <c r="I4" s="186"/>
+      <c r="J4" s="186"/>
+      <c r="K4" s="186"/>
+      <c r="L4" s="185"/>
+      <c r="M4" s="186"/>
+      <c r="N4" s="186"/>
+      <c r="O4" s="186"/>
+      <c r="P4" s="186"/>
+      <c r="Q4" s="186"/>
+      <c r="R4" s="186"/>
+      <c r="S4" s="186"/>
+      <c r="T4" s="189"/>
+      <c r="U4" s="190"/>
+      <c r="V4" s="190"/>
+      <c r="W4" s="190"/>
+      <c r="X4" s="190"/>
+      <c r="Y4" s="190"/>
+      <c r="Z4" s="190"/>
+      <c r="AA4" s="190"/>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="160" t="s">
+      <c r="A5" s="167" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="140" t="s">
+      <c r="B5" s="157" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="187" t="s">
+      <c r="D5" s="174" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="188"/>
-      <c r="F5" s="188"/>
-      <c r="G5" s="189"/>
-      <c r="H5" s="176" t="s">
+      <c r="E5" s="175"/>
+      <c r="F5" s="175"/>
+      <c r="G5" s="176"/>
+      <c r="H5" s="177" t="s">
         <v>64</v>
       </c>
-      <c r="I5" s="177"/>
-      <c r="J5" s="177"/>
-      <c r="K5" s="177"/>
-      <c r="L5" s="176" t="s">
+      <c r="I5" s="178"/>
+      <c r="J5" s="178"/>
+      <c r="K5" s="178"/>
+      <c r="L5" s="177" t="s">
         <v>69</v>
       </c>
-      <c r="M5" s="177"/>
-      <c r="N5" s="177"/>
-      <c r="O5" s="177"/>
-      <c r="P5" s="172" t="s">
+      <c r="M5" s="178"/>
+      <c r="N5" s="178"/>
+      <c r="O5" s="178"/>
+      <c r="P5" s="193" t="s">
         <v>91</v>
       </c>
-      <c r="Q5" s="173"/>
-      <c r="R5" s="173"/>
-      <c r="S5" s="174"/>
-      <c r="T5" s="149" t="s">
+      <c r="Q5" s="194"/>
+      <c r="R5" s="194"/>
+      <c r="S5" s="195"/>
+      <c r="T5" s="163" t="s">
         <v>110</v>
       </c>
-      <c r="U5" s="149"/>
-      <c r="V5" s="149"/>
-      <c r="W5" s="149"/>
-      <c r="X5" s="149" t="s">
+      <c r="U5" s="163"/>
+      <c r="V5" s="163"/>
+      <c r="W5" s="163"/>
+      <c r="X5" s="163" t="s">
         <v>111</v>
       </c>
-      <c r="Y5" s="149"/>
-      <c r="Z5" s="149"/>
-      <c r="AA5" s="149"/>
+      <c r="Y5" s="163"/>
+      <c r="Z5" s="163"/>
+      <c r="AA5" s="163"/>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="161"/>
-      <c r="B6" s="141"/>
+      <c r="A6" s="168"/>
+      <c r="B6" s="158"/>
       <c r="C6" s="9" t="s">
         <v>50</v>
       </c>
@@ -8344,8 +8766,8 @@
       <c r="AA6" s="85"/>
     </row>
     <row r="7" spans="1:27">
-      <c r="A7" s="161"/>
-      <c r="B7" s="141"/>
+      <c r="A7" s="168"/>
+      <c r="B7" s="158"/>
       <c r="C7" s="9" t="s">
         <v>48</v>
       </c>
@@ -8383,8 +8805,8 @@
       <c r="AA7" s="85"/>
     </row>
     <row r="8" spans="1:27" ht="15" customHeight="1">
-      <c r="A8" s="162"/>
-      <c r="B8" s="142"/>
+      <c r="A8" s="169"/>
+      <c r="B8" s="159"/>
       <c r="C8" s="10" t="s">
         <v>49</v>
       </c>
@@ -10006,10 +10428,10 @@
       <c r="AA56" s="85"/>
     </row>
     <row r="57" spans="1:27">
-      <c r="A57" s="138" t="s">
+      <c r="A57" s="155" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="139"/>
+      <c r="B57" s="156"/>
       <c r="C57" s="13"/>
       <c r="D57" s="17">
         <f>COUNTIF(D9:D56,"A")</f>
@@ -10109,10 +10531,10 @@
       </c>
     </row>
     <row r="58" spans="1:27">
-      <c r="A58" s="135" t="s">
+      <c r="A58" s="153" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="136"/>
+      <c r="B58" s="154"/>
       <c r="C58" s="13"/>
       <c r="D58" s="17">
         <f>(48-D57)</f>
@@ -10213,12 +10635,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="T4:AA4"/>
+    <mergeCell ref="L1:Z1"/>
+    <mergeCell ref="L2:Z2"/>
+    <mergeCell ref="L3:Z3"/>
+    <mergeCell ref="L4:S4"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="T5:W5"/>
+    <mergeCell ref="P5:S5"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="A3:C4"/>
@@ -10229,15 +10654,12 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="F3:I3"/>
-    <mergeCell ref="L5:O5"/>
-    <mergeCell ref="T4:AA4"/>
-    <mergeCell ref="L1:Z1"/>
-    <mergeCell ref="L2:Z2"/>
-    <mergeCell ref="L3:Z3"/>
-    <mergeCell ref="L4:S4"/>
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="T5:W5"/>
-    <mergeCell ref="P5:S5"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="A57:B57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -10248,8 +10670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10262,30 +10684,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="191" t="s">
+      <c r="A1" s="196" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="191"/>
-      <c r="C1" s="191"/>
-      <c r="D1" s="191"/>
+      <c r="B1" s="196"/>
+      <c r="C1" s="196"/>
+      <c r="D1" s="196"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="192" t="s">
+      <c r="A2" s="197" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="192"/>
-      <c r="C2" s="192"/>
-      <c r="D2" s="192"/>
+      <c r="B2" s="197"/>
+      <c r="C2" s="197"/>
+      <c r="D2" s="197"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="192" t="s">
-        <v>183</v>
-      </c>
-      <c r="B3" s="192"/>
-      <c r="C3" s="192"/>
-      <c r="D3" s="192"/>
-    </row>
-    <row r="4" spans="1:4" s="74" customFormat="1" ht="28.5">
+      <c r="A3" s="197" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" s="197"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+    </row>
+    <row r="4" spans="1:4" s="74" customFormat="1">
       <c r="A4" s="72" t="s">
         <v>93</v>
       </c>
@@ -10313,7 +10735,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="74" customFormat="1">
+    <row r="6" spans="1:4" s="74" customFormat="1" ht="28.5">
       <c r="A6" s="72" t="s">
         <v>96</v>
       </c>
@@ -10323,8 +10745,8 @@
       <c r="C6" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="75">
-        <v>43644</v>
+      <c r="D6" s="133">
+        <v>43651</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -10348,11 +10770,11 @@
       <c r="B8" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="61">
-        <v>14</v>
-      </c>
-      <c r="D8" s="195" t="s">
-        <v>184</v>
+      <c r="C8" s="62" t="s">
+        <v>189</v>
+      </c>
+      <c r="D8" s="132" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="74" customFormat="1">
@@ -10363,9 +10785,9 @@
         <v>2</v>
       </c>
       <c r="C9" s="62">
-        <v>10</v>
-      </c>
-      <c r="D9" s="195" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="130" t="s">
         <v>184</v>
       </c>
     </row>
@@ -10377,9 +10799,9 @@
         <v>3</v>
       </c>
       <c r="C10" s="61">
-        <v>14</v>
-      </c>
-      <c r="D10" s="195" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="130" t="s">
         <v>184</v>
       </c>
     </row>
@@ -10391,9 +10813,9 @@
         <v>102</v>
       </c>
       <c r="C11" s="61">
-        <v>12</v>
-      </c>
-      <c r="D11" s="195" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="130" t="s">
         <v>184</v>
       </c>
     </row>
@@ -10405,10 +10827,10 @@
         <v>5</v>
       </c>
       <c r="C12" s="61">
-        <v>14</v>
-      </c>
-      <c r="D12" s="195" t="s">
-        <v>184</v>
+        <v>22</v>
+      </c>
+      <c r="D12" s="131" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="74" customFormat="1">
@@ -10419,10 +10841,10 @@
         <v>6</v>
       </c>
       <c r="C13" s="61">
-        <v>11</v>
-      </c>
-      <c r="D13" s="195" t="s">
-        <v>184</v>
+        <v>21</v>
+      </c>
+      <c r="D13" s="131" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="74" customFormat="1">
@@ -10433,9 +10855,9 @@
         <v>7</v>
       </c>
       <c r="C14" s="61">
-        <v>15</v>
-      </c>
-      <c r="D14" s="196" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="131" t="s">
         <v>185</v>
       </c>
     </row>
@@ -10447,10 +10869,10 @@
         <v>8</v>
       </c>
       <c r="C15" s="61">
-        <v>14</v>
-      </c>
-      <c r="D15" s="195" t="s">
-        <v>184</v>
+        <v>22</v>
+      </c>
+      <c r="D15" s="131" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="74" customFormat="1">
@@ -10460,11 +10882,11 @@
       <c r="B16" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="62" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="197" t="s">
-        <v>186</v>
+      <c r="C16" s="62">
+        <v>5</v>
+      </c>
+      <c r="D16" s="130" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="74" customFormat="1">
@@ -10475,10 +10897,10 @@
         <v>9</v>
       </c>
       <c r="C17" s="61">
-        <v>12</v>
-      </c>
-      <c r="D17" s="195" t="s">
-        <v>184</v>
+        <v>21</v>
+      </c>
+      <c r="D17" s="131" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="74" customFormat="1">
@@ -10489,9 +10911,9 @@
         <v>10</v>
       </c>
       <c r="C18" s="61">
-        <v>17</v>
-      </c>
-      <c r="D18" s="196" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="131" t="s">
         <v>185</v>
       </c>
     </row>
@@ -10503,9 +10925,9 @@
         <v>11</v>
       </c>
       <c r="C19" s="61">
-        <v>19</v>
-      </c>
-      <c r="D19" s="196" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="131" t="s">
         <v>185</v>
       </c>
     </row>
@@ -10517,9 +10939,9 @@
         <v>12</v>
       </c>
       <c r="C20" s="61">
-        <v>14</v>
-      </c>
-      <c r="D20" s="195" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="130" t="s">
         <v>184</v>
       </c>
     </row>
@@ -10531,10 +10953,10 @@
         <v>13</v>
       </c>
       <c r="C21" s="61">
-        <v>11</v>
-      </c>
-      <c r="D21" s="195" t="s">
-        <v>184</v>
+        <v>19</v>
+      </c>
+      <c r="D21" s="131" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="74" customFormat="1">
@@ -10545,9 +10967,9 @@
         <v>14</v>
       </c>
       <c r="C22" s="61">
-        <v>8</v>
-      </c>
-      <c r="D22" s="195" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="130" t="s">
         <v>184</v>
       </c>
     </row>
@@ -10559,9 +10981,9 @@
         <v>15</v>
       </c>
       <c r="C23" s="61">
-        <v>11</v>
-      </c>
-      <c r="D23" s="195" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="130" t="s">
         <v>184</v>
       </c>
     </row>
@@ -10573,10 +10995,10 @@
         <v>16</v>
       </c>
       <c r="C24" s="61">
-        <v>12</v>
-      </c>
-      <c r="D24" s="195" t="s">
-        <v>184</v>
+        <v>22</v>
+      </c>
+      <c r="D24" s="131" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="74" customFormat="1">
@@ -10587,10 +11009,10 @@
         <v>17</v>
       </c>
       <c r="C25" s="61">
-        <v>7</v>
-      </c>
-      <c r="D25" s="195" t="s">
-        <v>184</v>
+        <v>19</v>
+      </c>
+      <c r="D25" s="131" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="74" customFormat="1">
@@ -10601,10 +11023,10 @@
         <v>18</v>
       </c>
       <c r="C26" s="61">
-        <v>12</v>
-      </c>
-      <c r="D26" s="195" t="s">
-        <v>184</v>
+        <v>18</v>
+      </c>
+      <c r="D26" s="131" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="74" customFormat="1">
@@ -10615,9 +11037,9 @@
         <v>19</v>
       </c>
       <c r="C27" s="61">
-        <v>15</v>
-      </c>
-      <c r="D27" s="196" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="131" t="s">
         <v>185</v>
       </c>
     </row>
@@ -10629,9 +11051,9 @@
         <v>20</v>
       </c>
       <c r="C28" s="61">
-        <v>3</v>
-      </c>
-      <c r="D28" s="195" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="130" t="s">
         <v>184</v>
       </c>
     </row>
@@ -10643,9 +11065,9 @@
         <v>21</v>
       </c>
       <c r="C29" s="61">
-        <v>16</v>
-      </c>
-      <c r="D29" s="196" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="131" t="s">
         <v>185</v>
       </c>
     </row>
@@ -10657,10 +11079,10 @@
         <v>22</v>
       </c>
       <c r="C30" s="61">
-        <v>12</v>
-      </c>
-      <c r="D30" s="195" t="s">
-        <v>184</v>
+        <v>19</v>
+      </c>
+      <c r="D30" s="131" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="74" customFormat="1">
@@ -10671,10 +11093,10 @@
         <v>23</v>
       </c>
       <c r="C31" s="61">
-        <v>13</v>
-      </c>
-      <c r="D31" s="195" t="s">
-        <v>184</v>
+        <v>19</v>
+      </c>
+      <c r="D31" s="131" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="74" customFormat="1">
@@ -10685,9 +11107,9 @@
         <v>24</v>
       </c>
       <c r="C32" s="61">
-        <v>9</v>
-      </c>
-      <c r="D32" s="195" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="130" t="s">
         <v>184</v>
       </c>
     </row>
@@ -10699,9 +11121,9 @@
         <v>25</v>
       </c>
       <c r="C33" s="61">
-        <v>22</v>
-      </c>
-      <c r="D33" s="196" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="131" t="s">
         <v>185</v>
       </c>
     </row>
@@ -10713,9 +11135,9 @@
         <v>26</v>
       </c>
       <c r="C34" s="61">
-        <v>3</v>
-      </c>
-      <c r="D34" s="195" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="130" t="s">
         <v>184</v>
       </c>
     </row>
@@ -10727,9 +11149,9 @@
         <v>27</v>
       </c>
       <c r="C35" s="61">
-        <v>22</v>
-      </c>
-      <c r="D35" s="196" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="131" t="s">
         <v>185</v>
       </c>
     </row>
@@ -10741,9 +11163,9 @@
         <v>28</v>
       </c>
       <c r="C36" s="61">
-        <v>21</v>
-      </c>
-      <c r="D36" s="196" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="131" t="s">
         <v>185</v>
       </c>
     </row>
@@ -10757,7 +11179,7 @@
       <c r="C37" s="61">
         <v>4</v>
       </c>
-      <c r="D37" s="195" t="s">
+      <c r="D37" s="130" t="s">
         <v>184</v>
       </c>
     </row>
@@ -10769,9 +11191,9 @@
         <v>30</v>
       </c>
       <c r="C38" s="61">
-        <v>21</v>
-      </c>
-      <c r="D38" s="196" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="131" t="s">
         <v>185</v>
       </c>
     </row>
@@ -10785,7 +11207,7 @@
       <c r="C39" s="61">
         <v>20</v>
       </c>
-      <c r="D39" s="196" t="s">
+      <c r="D39" s="131" t="s">
         <v>185</v>
       </c>
     </row>
@@ -10797,9 +11219,9 @@
         <v>32</v>
       </c>
       <c r="C40" s="61">
-        <v>11</v>
-      </c>
-      <c r="D40" s="195" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="130" t="s">
         <v>184</v>
       </c>
     </row>
@@ -10811,9 +11233,9 @@
         <v>33</v>
       </c>
       <c r="C41" s="61">
-        <v>16</v>
-      </c>
-      <c r="D41" s="196" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="131" t="s">
         <v>185</v>
       </c>
     </row>
@@ -10825,10 +11247,10 @@
         <v>34</v>
       </c>
       <c r="C42" s="61">
-        <v>14</v>
-      </c>
-      <c r="D42" s="195" t="s">
-        <v>184</v>
+        <v>18</v>
+      </c>
+      <c r="D42" s="131" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="74" customFormat="1">
@@ -10838,11 +11260,11 @@
       <c r="B43" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="62" t="s">
-        <v>56</v>
-      </c>
-      <c r="D43" s="197" t="s">
-        <v>186</v>
+      <c r="C43" s="62">
+        <v>14</v>
+      </c>
+      <c r="D43" s="130" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="74" customFormat="1">
@@ -10853,10 +11275,10 @@
         <v>36</v>
       </c>
       <c r="C44" s="61">
-        <v>11</v>
-      </c>
-      <c r="D44" s="195" t="s">
-        <v>184</v>
+        <v>19</v>
+      </c>
+      <c r="D44" s="131" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="74" customFormat="1">
@@ -10867,10 +11289,10 @@
         <v>37</v>
       </c>
       <c r="C45" s="61">
-        <v>6</v>
-      </c>
-      <c r="D45" s="195" t="s">
-        <v>184</v>
+        <v>18</v>
+      </c>
+      <c r="D45" s="131" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="74" customFormat="1">
@@ -10881,9 +11303,9 @@
         <v>38</v>
       </c>
       <c r="C46" s="61">
-        <v>9</v>
-      </c>
-      <c r="D46" s="195" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="130" t="s">
         <v>184</v>
       </c>
     </row>
@@ -10895,9 +11317,9 @@
         <v>39</v>
       </c>
       <c r="C47" s="61">
-        <v>13</v>
-      </c>
-      <c r="D47" s="195" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="130" t="s">
         <v>184</v>
       </c>
     </row>
@@ -10909,10 +11331,10 @@
         <v>40</v>
       </c>
       <c r="C48" s="61">
-        <v>1</v>
-      </c>
-      <c r="D48" s="195" t="s">
-        <v>184</v>
+        <v>19</v>
+      </c>
+      <c r="D48" s="131" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="74" customFormat="1">
@@ -10923,9 +11345,9 @@
         <v>41</v>
       </c>
       <c r="C49" s="61">
-        <v>17</v>
-      </c>
-      <c r="D49" s="196" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" s="131" t="s">
         <v>185</v>
       </c>
     </row>
@@ -10937,9 +11359,9 @@
         <v>42</v>
       </c>
       <c r="C50" s="61">
-        <v>24</v>
-      </c>
-      <c r="D50" s="196" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="131" t="s">
         <v>185</v>
       </c>
     </row>
@@ -10951,9 +11373,9 @@
         <v>43</v>
       </c>
       <c r="C51" s="61">
-        <v>19</v>
-      </c>
-      <c r="D51" s="196" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="131" t="s">
         <v>185</v>
       </c>
     </row>
@@ -10965,10 +11387,10 @@
         <v>44</v>
       </c>
       <c r="C52" s="61">
-        <v>9</v>
-      </c>
-      <c r="D52" s="195" t="s">
-        <v>184</v>
+        <v>18</v>
+      </c>
+      <c r="D52" s="131" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="74" customFormat="1">
@@ -10979,9 +11401,9 @@
         <v>45</v>
       </c>
       <c r="C53" s="61">
-        <v>17</v>
-      </c>
-      <c r="D53" s="196" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="131" t="s">
         <v>185</v>
       </c>
     </row>
@@ -10993,9 +11415,9 @@
         <v>46</v>
       </c>
       <c r="C54" s="61">
-        <v>17</v>
-      </c>
-      <c r="D54" s="196" t="s">
+        <v>21</v>
+      </c>
+      <c r="D54" s="131" t="s">
         <v>185</v>
       </c>
     </row>
@@ -11007,9 +11429,9 @@
         <v>47</v>
       </c>
       <c r="C55" s="63">
-        <v>17</v>
-      </c>
-      <c r="D55" s="196" t="s">
+        <v>21</v>
+      </c>
+      <c r="D55" s="131" t="s">
         <v>185</v>
       </c>
     </row>
@@ -11021,10 +11443,10 @@
         <v>181</v>
       </c>
       <c r="C56" s="63">
-        <v>12</v>
-      </c>
-      <c r="D56" s="195" t="s">
-        <v>184</v>
+        <v>18</v>
+      </c>
+      <c r="D56" s="131" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="74" customFormat="1">
@@ -11035,9 +11457,9 @@
         <v>182</v>
       </c>
       <c r="C57" s="61">
-        <v>17</v>
-      </c>
-      <c r="D57" s="196" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57" s="131" t="s">
         <v>185</v>
       </c>
     </row>
@@ -11048,7 +11470,820 @@
     <mergeCell ref="A3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:C57">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="lessThan">
+      <formula>18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:C57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" style="60" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="60" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="60" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" style="70" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="60"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="196" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="196"/>
+      <c r="C1" s="196"/>
+      <c r="D1" s="196"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="197" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="197"/>
+      <c r="C2" s="197"/>
+      <c r="D2" s="197"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="197" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="197"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
+    </row>
+    <row r="4" spans="1:4" s="74" customFormat="1">
+      <c r="A4" s="72" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="71" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="74" customFormat="1" ht="28.5">
+      <c r="A5" s="72" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="71" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" s="73" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="71" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="74" customFormat="1" ht="28.5">
+      <c r="A6" s="72" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="71" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="75">
+        <v>43644</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="65" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="74" customFormat="1">
+      <c r="A8" s="57">
+        <v>1</v>
+      </c>
+      <c r="B8" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="61">
+        <v>14</v>
+      </c>
+      <c r="D8" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="74" customFormat="1">
+      <c r="A9" s="57">
+        <v>2</v>
+      </c>
+      <c r="B9" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="62">
+        <v>10</v>
+      </c>
+      <c r="D9" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="74" customFormat="1">
+      <c r="A10" s="57">
+        <v>3</v>
+      </c>
+      <c r="B10" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="61">
+        <v>14</v>
+      </c>
+      <c r="D10" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="74" customFormat="1">
+      <c r="A11" s="57">
+        <v>4</v>
+      </c>
+      <c r="B11" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="61">
+        <v>12</v>
+      </c>
+      <c r="D11" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="74" customFormat="1">
+      <c r="A12" s="57">
+        <v>5</v>
+      </c>
+      <c r="B12" s="76" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="61">
+        <v>14</v>
+      </c>
+      <c r="D12" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="74" customFormat="1">
+      <c r="A13" s="57">
+        <v>6</v>
+      </c>
+      <c r="B13" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="61">
+        <v>11</v>
+      </c>
+      <c r="D13" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="74" customFormat="1">
+      <c r="A14" s="57">
+        <v>7</v>
+      </c>
+      <c r="B14" s="76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="61">
+        <v>15</v>
+      </c>
+      <c r="D14" s="131" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="74" customFormat="1">
+      <c r="A15" s="57">
+        <v>8</v>
+      </c>
+      <c r="B15" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="61">
+        <v>14</v>
+      </c>
+      <c r="D15" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="74" customFormat="1">
+      <c r="A16" s="57">
+        <v>9</v>
+      </c>
+      <c r="B16" s="76" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="132" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="74" customFormat="1">
+      <c r="A17" s="57">
+        <v>10</v>
+      </c>
+      <c r="B17" s="76" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="61">
+        <v>12</v>
+      </c>
+      <c r="D17" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="74" customFormat="1">
+      <c r="A18" s="57">
+        <v>11</v>
+      </c>
+      <c r="B18" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="61">
+        <v>17</v>
+      </c>
+      <c r="D18" s="131" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="74" customFormat="1">
+      <c r="A19" s="57">
+        <v>12</v>
+      </c>
+      <c r="B19" s="76" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="61">
+        <v>19</v>
+      </c>
+      <c r="D19" s="131" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="74" customFormat="1">
+      <c r="A20" s="57">
+        <v>13</v>
+      </c>
+      <c r="B20" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="61">
+        <v>14</v>
+      </c>
+      <c r="D20" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="74" customFormat="1">
+      <c r="A21" s="57">
+        <v>14</v>
+      </c>
+      <c r="B21" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="61">
+        <v>11</v>
+      </c>
+      <c r="D21" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="74" customFormat="1">
+      <c r="A22" s="57">
+        <v>15</v>
+      </c>
+      <c r="B22" s="78" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="61">
+        <v>8</v>
+      </c>
+      <c r="D22" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="74" customFormat="1">
+      <c r="A23" s="57">
+        <v>16</v>
+      </c>
+      <c r="B23" s="76" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="61">
+        <v>11</v>
+      </c>
+      <c r="D23" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="74" customFormat="1">
+      <c r="A24" s="57">
+        <v>17</v>
+      </c>
+      <c r="B24" s="76" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="61">
+        <v>12</v>
+      </c>
+      <c r="D24" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="74" customFormat="1">
+      <c r="A25" s="57">
+        <v>18</v>
+      </c>
+      <c r="B25" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="61">
+        <v>7</v>
+      </c>
+      <c r="D25" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="74" customFormat="1">
+      <c r="A26" s="57">
+        <v>19</v>
+      </c>
+      <c r="B26" s="76" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="61">
+        <v>12</v>
+      </c>
+      <c r="D26" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="74" customFormat="1">
+      <c r="A27" s="57">
+        <v>20</v>
+      </c>
+      <c r="B27" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="61">
+        <v>15</v>
+      </c>
+      <c r="D27" s="131" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="74" customFormat="1">
+      <c r="A28" s="57">
+        <v>21</v>
+      </c>
+      <c r="B28" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="61">
+        <v>3</v>
+      </c>
+      <c r="D28" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="74" customFormat="1">
+      <c r="A29" s="57">
+        <v>22</v>
+      </c>
+      <c r="B29" s="76" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="61">
+        <v>16</v>
+      </c>
+      <c r="D29" s="131" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="74" customFormat="1">
+      <c r="A30" s="57">
+        <v>23</v>
+      </c>
+      <c r="B30" s="79" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="61">
+        <v>12</v>
+      </c>
+      <c r="D30" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="74" customFormat="1">
+      <c r="A31" s="57">
+        <v>24</v>
+      </c>
+      <c r="B31" s="80" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="61">
+        <v>13</v>
+      </c>
+      <c r="D31" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="74" customFormat="1">
+      <c r="A32" s="57">
+        <v>25</v>
+      </c>
+      <c r="B32" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="61">
+        <v>9</v>
+      </c>
+      <c r="D32" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="74" customFormat="1">
+      <c r="A33" s="57">
+        <v>26</v>
+      </c>
+      <c r="B33" s="76" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="61">
+        <v>22</v>
+      </c>
+      <c r="D33" s="131" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="74" customFormat="1">
+      <c r="A34" s="57">
+        <v>27</v>
+      </c>
+      <c r="B34" s="80" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="61">
+        <v>3</v>
+      </c>
+      <c r="D34" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="74" customFormat="1">
+      <c r="A35" s="57">
+        <v>28</v>
+      </c>
+      <c r="B35" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="61">
+        <v>22</v>
+      </c>
+      <c r="D35" s="131" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="74" customFormat="1">
+      <c r="A36" s="57">
+        <v>29</v>
+      </c>
+      <c r="B36" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" s="61">
+        <v>21</v>
+      </c>
+      <c r="D36" s="131" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="74" customFormat="1">
+      <c r="A37" s="57">
+        <v>30</v>
+      </c>
+      <c r="B37" s="76" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="61">
+        <v>4</v>
+      </c>
+      <c r="D37" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="74" customFormat="1">
+      <c r="A38" s="57">
+        <v>31</v>
+      </c>
+      <c r="B38" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="61">
+        <v>21</v>
+      </c>
+      <c r="D38" s="131" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="74" customFormat="1">
+      <c r="A39" s="57">
+        <v>32</v>
+      </c>
+      <c r="B39" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" s="61">
+        <v>20</v>
+      </c>
+      <c r="D39" s="131" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="74" customFormat="1">
+      <c r="A40" s="57">
+        <v>33</v>
+      </c>
+      <c r="B40" s="76" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="61">
+        <v>11</v>
+      </c>
+      <c r="D40" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="74" customFormat="1">
+      <c r="A41" s="57">
+        <v>34</v>
+      </c>
+      <c r="B41" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="61">
+        <v>16</v>
+      </c>
+      <c r="D41" s="131" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="74" customFormat="1">
+      <c r="A42" s="57">
+        <v>35</v>
+      </c>
+      <c r="B42" s="76" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="61">
+        <v>14</v>
+      </c>
+      <c r="D42" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="74" customFormat="1">
+      <c r="A43" s="57">
+        <v>36</v>
+      </c>
+      <c r="B43" s="76" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="132" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="74" customFormat="1">
+      <c r="A44" s="57">
+        <v>37</v>
+      </c>
+      <c r="B44" s="78" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="61">
+        <v>11</v>
+      </c>
+      <c r="D44" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="74" customFormat="1">
+      <c r="A45" s="57">
+        <v>38</v>
+      </c>
+      <c r="B45" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="61">
+        <v>6</v>
+      </c>
+      <c r="D45" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="74" customFormat="1">
+      <c r="A46" s="57">
+        <v>39</v>
+      </c>
+      <c r="B46" s="80" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="61">
+        <v>9</v>
+      </c>
+      <c r="D46" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="74" customFormat="1">
+      <c r="A47" s="57">
+        <v>40</v>
+      </c>
+      <c r="B47" s="76" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" s="61">
+        <v>13</v>
+      </c>
+      <c r="D47" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="74" customFormat="1">
+      <c r="A48" s="57">
+        <v>41</v>
+      </c>
+      <c r="B48" s="76" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="61">
+        <v>1</v>
+      </c>
+      <c r="D48" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="74" customFormat="1">
+      <c r="A49" s="57">
+        <v>42</v>
+      </c>
+      <c r="B49" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" s="61">
+        <v>17</v>
+      </c>
+      <c r="D49" s="131" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="74" customFormat="1">
+      <c r="A50" s="57">
+        <v>43</v>
+      </c>
+      <c r="B50" s="78" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="61">
+        <v>24</v>
+      </c>
+      <c r="D50" s="131" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="74" customFormat="1">
+      <c r="A51" s="57">
+        <v>44</v>
+      </c>
+      <c r="B51" s="78" t="s">
+        <v>43</v>
+      </c>
+      <c r="C51" s="61">
+        <v>19</v>
+      </c>
+      <c r="D51" s="131" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="74" customFormat="1">
+      <c r="A52" s="57">
+        <v>45</v>
+      </c>
+      <c r="B52" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" s="61">
+        <v>9</v>
+      </c>
+      <c r="D52" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="74" customFormat="1">
+      <c r="A53" s="57">
+        <v>46</v>
+      </c>
+      <c r="B53" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53" s="61">
+        <v>17</v>
+      </c>
+      <c r="D53" s="131" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="74" customFormat="1">
+      <c r="A54" s="57">
+        <v>47</v>
+      </c>
+      <c r="B54" s="76" t="s">
+        <v>46</v>
+      </c>
+      <c r="C54" s="61">
+        <v>17</v>
+      </c>
+      <c r="D54" s="131" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="74" customFormat="1">
+      <c r="A55" s="55">
+        <v>48</v>
+      </c>
+      <c r="B55" s="81" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" s="63">
+        <v>17</v>
+      </c>
+      <c r="D55" s="131" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="74" customFormat="1">
+      <c r="A56" s="55">
+        <v>49</v>
+      </c>
+      <c r="B56" s="81" t="s">
+        <v>181</v>
+      </c>
+      <c r="C56" s="63">
+        <v>12</v>
+      </c>
+      <c r="D56" s="130" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="74" customFormat="1">
+      <c r="A57" s="57">
+        <v>50</v>
+      </c>
+      <c r="B57" s="76" t="s">
+        <v>182</v>
+      </c>
+      <c r="C57" s="61">
+        <v>17</v>
+      </c>
+      <c r="D57" s="131" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C8:C57">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="lessThan">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11057,7 +12292,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D63"/>
   <sheetViews>
@@ -11075,28 +12310,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="191" t="s">
+      <c r="A1" s="196" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="191"/>
-      <c r="C1" s="191"/>
-      <c r="D1" s="191"/>
+      <c r="B1" s="196"/>
+      <c r="C1" s="196"/>
+      <c r="D1" s="196"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="192" t="s">
+      <c r="A2" s="197" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="192"/>
-      <c r="C2" s="192"/>
-      <c r="D2" s="192"/>
+      <c r="B2" s="197"/>
+      <c r="C2" s="197"/>
+      <c r="D2" s="197"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="192" t="s">
+      <c r="A3" s="197" t="s">
         <v>178</v>
       </c>
-      <c r="B3" s="192"/>
-      <c r="C3" s="192"/>
-      <c r="D3" s="192"/>
+      <c r="B3" s="197"/>
+      <c r="C3" s="197"/>
+      <c r="D3" s="197"/>
     </row>
     <row r="4" spans="1:4" s="74" customFormat="1" ht="28.5">
       <c r="A4" s="72" t="s">
@@ -11633,41 +12868,41 @@
       <c r="D55" s="63"/>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="190" t="s">
+      <c r="A56" s="198" t="s">
         <v>103</v>
       </c>
-      <c r="B56" s="190"/>
-      <c r="C56" s="190"/>
+      <c r="B56" s="198"/>
+      <c r="C56" s="198"/>
       <c r="D56" s="66">
         <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="190" t="s">
+      <c r="A57" s="198" t="s">
         <v>104</v>
       </c>
-      <c r="B57" s="190"/>
-      <c r="C57" s="190"/>
+      <c r="B57" s="198"/>
+      <c r="C57" s="198"/>
       <c r="D57" s="67">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="190" t="s">
+      <c r="A58" s="198" t="s">
         <v>105</v>
       </c>
-      <c r="B58" s="190"/>
-      <c r="C58" s="190"/>
+      <c r="B58" s="198"/>
+      <c r="C58" s="198"/>
       <c r="D58" s="67">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="190" t="s">
+      <c r="A59" s="198" t="s">
         <v>106</v>
       </c>
-      <c r="B59" s="190"/>
-      <c r="C59" s="190"/>
+      <c r="B59" s="198"/>
+      <c r="C59" s="198"/>
       <c r="D59" s="67">
         <v>92</v>
       </c>
@@ -11713,7 +12948,7 @@
     <mergeCell ref="A3:D3"/>
   </mergeCells>
   <conditionalFormatting sqref="C25:C55 C8:C23">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11722,7 +12957,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D63"/>
   <sheetViews>
@@ -11740,28 +12975,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="193" t="s">
+      <c r="A1" s="199" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="193"/>
-      <c r="C1" s="193"/>
-      <c r="D1" s="193"/>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
     </row>
     <row r="2" spans="1:4" ht="15.75">
-      <c r="A2" s="194" t="s">
+      <c r="A2" s="200" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="194"/>
-      <c r="C2" s="194"/>
-      <c r="D2" s="194"/>
+      <c r="B2" s="200"/>
+      <c r="C2" s="200"/>
+      <c r="D2" s="200"/>
     </row>
     <row r="3" spans="1:4" ht="15.75">
-      <c r="A3" s="194" t="s">
+      <c r="A3" s="200" t="s">
         <v>180</v>
       </c>
-      <c r="B3" s="194"/>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
+      <c r="B3" s="200"/>
+      <c r="C3" s="200"/>
+      <c r="D3" s="200"/>
     </row>
     <row r="4" spans="1:4" s="74" customFormat="1" ht="31.5">
       <c r="A4" s="89" t="s">
@@ -12490,41 +13725,41 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75">
-      <c r="A56" s="159" t="s">
+      <c r="A56" s="165" t="s">
         <v>103</v>
       </c>
-      <c r="B56" s="159"/>
-      <c r="C56" s="159"/>
+      <c r="B56" s="165"/>
+      <c r="C56" s="165"/>
       <c r="D56" s="101">
         <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75">
-      <c r="A57" s="159" t="s">
+      <c r="A57" s="165" t="s">
         <v>104</v>
       </c>
-      <c r="B57" s="159"/>
-      <c r="C57" s="159"/>
+      <c r="B57" s="165"/>
+      <c r="C57" s="165"/>
       <c r="D57" s="102">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75">
-      <c r="A58" s="159" t="s">
+      <c r="A58" s="165" t="s">
         <v>105</v>
       </c>
-      <c r="B58" s="159"/>
-      <c r="C58" s="159"/>
+      <c r="B58" s="165"/>
+      <c r="C58" s="165"/>
       <c r="D58" s="102">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75">
-      <c r="A59" s="159" t="s">
+      <c r="A59" s="165" t="s">
         <v>106</v>
       </c>
-      <c r="B59" s="159"/>
-      <c r="C59" s="159"/>
+      <c r="B59" s="165"/>
+      <c r="C59" s="165"/>
       <c r="D59" s="122">
         <f>(D56/48)*100</f>
         <v>97.916666666666657</v>
@@ -12572,12 +13807,12 @@
     <mergeCell ref="A58:C58"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:C55">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C55">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="lessThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12586,7 +13821,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E52"/>
   <sheetViews>
@@ -12604,31 +13839,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75">
-      <c r="A1" s="193" t="s">
+      <c r="A1" s="199" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="193"/>
-      <c r="C1" s="193"/>
-      <c r="D1" s="193"/>
-      <c r="E1" s="193"/>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
+      <c r="E1" s="199"/>
     </row>
     <row r="2" spans="1:5" ht="15.75">
-      <c r="A2" s="194" t="s">
+      <c r="A2" s="200" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="194"/>
-      <c r="C2" s="194"/>
-      <c r="D2" s="194"/>
-      <c r="E2" s="194"/>
+      <c r="B2" s="200"/>
+      <c r="C2" s="200"/>
+      <c r="D2" s="200"/>
+      <c r="E2" s="200"/>
     </row>
     <row r="3" spans="1:5" ht="15.75">
-      <c r="A3" s="194" t="s">
+      <c r="A3" s="200" t="s">
         <v>163</v>
       </c>
-      <c r="B3" s="194"/>
-      <c r="C3" s="194"/>
-      <c r="D3" s="194"/>
-      <c r="E3" s="194"/>
+      <c r="B3" s="200"/>
+      <c r="C3" s="200"/>
+      <c r="D3" s="200"/>
+      <c r="E3" s="200"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
       <c r="A4" s="116" t="s">
@@ -13390,17 +14625,583 @@
     <mergeCell ref="A3:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:D52">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"Not Submitted"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"Not Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="1.04" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" style="60" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="60" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="60" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" style="70" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="60"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="201" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="201"/>
+      <c r="C1" s="201"/>
+      <c r="D1" s="201"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="202" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="202"/>
+      <c r="C2" s="202"/>
+      <c r="D2" s="202"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="202" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="202"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="202"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="56" t="s">
+        <v>192</v>
+      </c>
+      <c r="D4" s="65" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="74" customFormat="1">
+      <c r="A5" s="57">
+        <v>1</v>
+      </c>
+      <c r="B5" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="134"/>
+      <c r="D5" s="134"/>
+    </row>
+    <row r="6" spans="1:4" s="74" customFormat="1">
+      <c r="A6" s="57">
+        <v>2</v>
+      </c>
+      <c r="B6" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="134"/>
+      <c r="D6" s="134"/>
+    </row>
+    <row r="7" spans="1:4" s="74" customFormat="1">
+      <c r="A7" s="57">
+        <v>3</v>
+      </c>
+      <c r="B7" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="134"/>
+      <c r="D7" s="134"/>
+    </row>
+    <row r="8" spans="1:4" s="74" customFormat="1">
+      <c r="A8" s="57">
+        <v>4</v>
+      </c>
+      <c r="B8" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="134"/>
+      <c r="D8" s="134"/>
+    </row>
+    <row r="9" spans="1:4" s="74" customFormat="1">
+      <c r="A9" s="57">
+        <v>5</v>
+      </c>
+      <c r="B9" s="76" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="134"/>
+      <c r="D9" s="134"/>
+    </row>
+    <row r="10" spans="1:4" s="74" customFormat="1">
+      <c r="A10" s="57">
+        <v>6</v>
+      </c>
+      <c r="B10" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="134"/>
+      <c r="D10" s="134"/>
+    </row>
+    <row r="11" spans="1:4" s="74" customFormat="1">
+      <c r="A11" s="57">
+        <v>7</v>
+      </c>
+      <c r="B11" s="76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="134"/>
+      <c r="D11" s="134"/>
+    </row>
+    <row r="12" spans="1:4" s="74" customFormat="1">
+      <c r="A12" s="57">
+        <v>8</v>
+      </c>
+      <c r="B12" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="134"/>
+      <c r="D12" s="134"/>
+    </row>
+    <row r="13" spans="1:4" s="74" customFormat="1">
+      <c r="A13" s="57">
+        <v>9</v>
+      </c>
+      <c r="B13" s="76" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="134"/>
+      <c r="D13" s="134"/>
+    </row>
+    <row r="14" spans="1:4" s="74" customFormat="1">
+      <c r="A14" s="57">
+        <v>10</v>
+      </c>
+      <c r="B14" s="76" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="134"/>
+      <c r="D14" s="134"/>
+    </row>
+    <row r="15" spans="1:4" s="74" customFormat="1">
+      <c r="A15" s="57">
+        <v>11</v>
+      </c>
+      <c r="B15" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="134"/>
+      <c r="D15" s="134"/>
+    </row>
+    <row r="16" spans="1:4" s="74" customFormat="1">
+      <c r="A16" s="57">
+        <v>12</v>
+      </c>
+      <c r="B16" s="76" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="134"/>
+      <c r="D16" s="134"/>
+    </row>
+    <row r="17" spans="1:4" s="74" customFormat="1">
+      <c r="A17" s="57">
+        <v>13</v>
+      </c>
+      <c r="B17" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="134"/>
+      <c r="D17" s="134"/>
+    </row>
+    <row r="18" spans="1:4" s="74" customFormat="1">
+      <c r="A18" s="57">
+        <v>14</v>
+      </c>
+      <c r="B18" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="134"/>
+      <c r="D18" s="134"/>
+    </row>
+    <row r="19" spans="1:4" s="74" customFormat="1">
+      <c r="A19" s="57">
+        <v>15</v>
+      </c>
+      <c r="B19" s="78" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="134"/>
+      <c r="D19" s="134"/>
+    </row>
+    <row r="20" spans="1:4" s="74" customFormat="1">
+      <c r="A20" s="57">
+        <v>16</v>
+      </c>
+      <c r="B20" s="76" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="134"/>
+      <c r="D20" s="134"/>
+    </row>
+    <row r="21" spans="1:4" s="74" customFormat="1">
+      <c r="A21" s="57">
+        <v>17</v>
+      </c>
+      <c r="B21" s="76" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="134"/>
+      <c r="D21" s="134"/>
+    </row>
+    <row r="22" spans="1:4" s="74" customFormat="1">
+      <c r="A22" s="57">
+        <v>18</v>
+      </c>
+      <c r="B22" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="134"/>
+      <c r="D22" s="134"/>
+    </row>
+    <row r="23" spans="1:4" s="74" customFormat="1">
+      <c r="A23" s="57">
+        <v>19</v>
+      </c>
+      <c r="B23" s="76" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="134"/>
+      <c r="D23" s="134"/>
+    </row>
+    <row r="24" spans="1:4" s="74" customFormat="1">
+      <c r="A24" s="57">
+        <v>20</v>
+      </c>
+      <c r="B24" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="134"/>
+      <c r="D24" s="134"/>
+    </row>
+    <row r="25" spans="1:4" s="74" customFormat="1">
+      <c r="A25" s="57">
+        <v>21</v>
+      </c>
+      <c r="B25" s="76" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="134"/>
+      <c r="D25" s="134"/>
+    </row>
+    <row r="26" spans="1:4" s="74" customFormat="1">
+      <c r="A26" s="57">
+        <v>22</v>
+      </c>
+      <c r="B26" s="76" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="134"/>
+      <c r="D26" s="134"/>
+    </row>
+    <row r="27" spans="1:4" s="74" customFormat="1">
+      <c r="A27" s="57">
+        <v>23</v>
+      </c>
+      <c r="B27" s="79" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="134"/>
+      <c r="D27" s="134"/>
+    </row>
+    <row r="28" spans="1:4" s="74" customFormat="1">
+      <c r="A28" s="57">
+        <v>24</v>
+      </c>
+      <c r="B28" s="80" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="134"/>
+      <c r="D28" s="134"/>
+    </row>
+    <row r="29" spans="1:4" s="74" customFormat="1">
+      <c r="A29" s="57">
+        <v>25</v>
+      </c>
+      <c r="B29" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="134"/>
+      <c r="D29" s="134"/>
+    </row>
+    <row r="30" spans="1:4" s="74" customFormat="1">
+      <c r="A30" s="57">
+        <v>26</v>
+      </c>
+      <c r="B30" s="76" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="134"/>
+      <c r="D30" s="134"/>
+    </row>
+    <row r="31" spans="1:4" s="74" customFormat="1">
+      <c r="A31" s="57">
+        <v>27</v>
+      </c>
+      <c r="B31" s="80" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="134"/>
+      <c r="D31" s="134"/>
+    </row>
+    <row r="32" spans="1:4" s="74" customFormat="1">
+      <c r="A32" s="57">
+        <v>28</v>
+      </c>
+      <c r="B32" s="76" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="134"/>
+      <c r="D32" s="134"/>
+    </row>
+    <row r="33" spans="1:4" s="74" customFormat="1">
+      <c r="A33" s="57">
+        <v>29</v>
+      </c>
+      <c r="B33" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="134"/>
+      <c r="D33" s="134"/>
+    </row>
+    <row r="34" spans="1:4" s="74" customFormat="1">
+      <c r="A34" s="57">
+        <v>30</v>
+      </c>
+      <c r="B34" s="76" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="134"/>
+      <c r="D34" s="134"/>
+    </row>
+    <row r="35" spans="1:4" s="74" customFormat="1">
+      <c r="A35" s="57">
+        <v>31</v>
+      </c>
+      <c r="B35" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="134"/>
+      <c r="D35" s="134"/>
+    </row>
+    <row r="36" spans="1:4" s="74" customFormat="1">
+      <c r="A36" s="57">
+        <v>32</v>
+      </c>
+      <c r="B36" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="134"/>
+      <c r="D36" s="134"/>
+    </row>
+    <row r="37" spans="1:4" s="74" customFormat="1">
+      <c r="A37" s="57">
+        <v>33</v>
+      </c>
+      <c r="B37" s="76" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="134"/>
+      <c r="D37" s="134"/>
+    </row>
+    <row r="38" spans="1:4" s="74" customFormat="1">
+      <c r="A38" s="57">
+        <v>34</v>
+      </c>
+      <c r="B38" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="134"/>
+      <c r="D38" s="134"/>
+    </row>
+    <row r="39" spans="1:4" s="74" customFormat="1">
+      <c r="A39" s="57">
+        <v>35</v>
+      </c>
+      <c r="B39" s="76" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="134"/>
+      <c r="D39" s="134"/>
+    </row>
+    <row r="40" spans="1:4" s="74" customFormat="1">
+      <c r="A40" s="57">
+        <v>36</v>
+      </c>
+      <c r="B40" s="76" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="134"/>
+      <c r="D40" s="134"/>
+    </row>
+    <row r="41" spans="1:4" s="74" customFormat="1">
+      <c r="A41" s="57">
+        <v>37</v>
+      </c>
+      <c r="B41" s="78" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="134"/>
+      <c r="D41" s="134"/>
+    </row>
+    <row r="42" spans="1:4" s="74" customFormat="1">
+      <c r="A42" s="57">
+        <v>38</v>
+      </c>
+      <c r="B42" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="134"/>
+      <c r="D42" s="134"/>
+    </row>
+    <row r="43" spans="1:4" s="74" customFormat="1">
+      <c r="A43" s="57">
+        <v>39</v>
+      </c>
+      <c r="B43" s="80" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="134"/>
+      <c r="D43" s="134"/>
+    </row>
+    <row r="44" spans="1:4" s="74" customFormat="1">
+      <c r="A44" s="57">
+        <v>40</v>
+      </c>
+      <c r="B44" s="76" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" s="134"/>
+      <c r="D44" s="134"/>
+    </row>
+    <row r="45" spans="1:4" s="74" customFormat="1">
+      <c r="A45" s="57">
+        <v>41</v>
+      </c>
+      <c r="B45" s="76" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" s="134"/>
+      <c r="D45" s="134"/>
+    </row>
+    <row r="46" spans="1:4" s="74" customFormat="1">
+      <c r="A46" s="57">
+        <v>42</v>
+      </c>
+      <c r="B46" s="76" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" s="134"/>
+      <c r="D46" s="134"/>
+    </row>
+    <row r="47" spans="1:4" s="74" customFormat="1">
+      <c r="A47" s="57">
+        <v>43</v>
+      </c>
+      <c r="B47" s="78" t="s">
+        <v>42</v>
+      </c>
+      <c r="C47" s="134"/>
+      <c r="D47" s="134"/>
+    </row>
+    <row r="48" spans="1:4" s="74" customFormat="1">
+      <c r="A48" s="57">
+        <v>44</v>
+      </c>
+      <c r="B48" s="78" t="s">
+        <v>43</v>
+      </c>
+      <c r="C48" s="134"/>
+      <c r="D48" s="134"/>
+    </row>
+    <row r="49" spans="1:4" s="74" customFormat="1">
+      <c r="A49" s="57">
+        <v>45</v>
+      </c>
+      <c r="B49" s="76" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" s="134"/>
+      <c r="D49" s="134"/>
+    </row>
+    <row r="50" spans="1:4" s="74" customFormat="1">
+      <c r="A50" s="57">
+        <v>46</v>
+      </c>
+      <c r="B50" s="76" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" s="134"/>
+      <c r="D50" s="134"/>
+    </row>
+    <row r="51" spans="1:4" s="74" customFormat="1">
+      <c r="A51" s="57">
+        <v>47</v>
+      </c>
+      <c r="B51" s="76" t="s">
+        <v>46</v>
+      </c>
+      <c r="C51" s="134"/>
+      <c r="D51" s="134"/>
+    </row>
+    <row r="52" spans="1:4" s="74" customFormat="1">
+      <c r="A52" s="55">
+        <v>48</v>
+      </c>
+      <c r="B52" s="81" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52" s="135"/>
+      <c r="D52" s="134"/>
+    </row>
+    <row r="53" spans="1:4" s="74" customFormat="1">
+      <c r="A53" s="55">
+        <v>49</v>
+      </c>
+      <c r="B53" s="81" t="s">
+        <v>181</v>
+      </c>
+      <c r="C53" s="135"/>
+      <c r="D53" s="134"/>
+    </row>
+    <row r="54" spans="1:4" s="74" customFormat="1">
+      <c r="A54" s="57">
+        <v>50</v>
+      </c>
+      <c r="B54" s="76" t="s">
+        <v>182</v>
+      </c>
+      <c r="C54" s="134"/>
+      <c r="D54" s="134"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>